<commit_message>
Filmes: Assistidos Madagascar 3 e Cinderela, Mudado Formato de Hora nas planilhas de cada produtora
</commit_message>
<xml_diff>
--- a/Filmes.xlsx
+++ b/Filmes.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Paulo\Documents\Planilhas\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D301E20-0E9A-4F41-8E59-6C642ED6CE19}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{92C2C1FC-6F10-48F3-BF7A-D14EE1D04B98}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{AC88744C-D9DF-4ECD-8B9A-C97C8CD0E4BD}"/>
   </bookViews>
@@ -61,7 +61,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="782" uniqueCount="256">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="783" uniqueCount="256">
   <si>
     <t>Nome do Filme</t>
   </si>
@@ -835,11 +835,12 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="4">
+  <numFmts count="5">
     <numFmt numFmtId="164" formatCode="0000"/>
     <numFmt numFmtId="165" formatCode="h:mm;@"/>
-    <numFmt numFmtId="167" formatCode="_-[$$-409]* #,##0.00_ ;_-[$$-409]* \-#,##0.00\ ;_-[$$-409]* &quot;-&quot;??_ ;_-@_ "/>
-    <numFmt numFmtId="168" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
+    <numFmt numFmtId="166" formatCode="_-[$$-409]* #,##0.00_ ;_-[$$-409]* \-#,##0.00\ ;_-[$$-409]* &quot;-&quot;??_ ;_-@_ "/>
+    <numFmt numFmtId="167" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
+    <numFmt numFmtId="170" formatCode="[h]:mm:ss;@"/>
   </numFmts>
   <fonts count="11" x14ac:knownFonts="1">
     <font>
@@ -1352,25 +1353,25 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="167" fontId="3" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="3" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="167" fontId="1" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="1" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="167" fontId="9" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="9" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="167" fontId="1" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="1" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="167" fontId="9" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="9" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="168" fontId="6" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="6" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="165" fontId="6" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1391,8 +1392,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="168" fontId="3" fillId="2" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="167" fontId="3" fillId="2" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -1406,6 +1407,28 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="3" fillId="2" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="0" fillId="3" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="167" fontId="3" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -1425,33 +1448,11 @@
     <xf numFmtId="0" fontId="10" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="168" fontId="3" fillId="2" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="168" fontId="3" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="170" fontId="3" fillId="2" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="168" fontId="3" fillId="2" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="168" fontId="0" fillId="3" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="168" fontId="3" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="170" fontId="3" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2028,8 +2029,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B5A731FE-9613-428C-993D-C03F78E1A52D}">
   <dimension ref="A1:AF201"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="T61" zoomScale="96" zoomScaleNormal="96" workbookViewId="0">
-      <selection activeCell="Y47" sqref="Y47"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="J17" zoomScale="96" zoomScaleNormal="96" workbookViewId="0">
+      <selection activeCell="V31" sqref="V31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2040,7 +2041,7 @@
     <col min="4" max="4" width="12.140625" style="6" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="15.42578125" style="6" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="7.140625" style="9" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="15.85546875" style="72" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.85546875" style="65" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="22.5703125" style="6" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="22.5703125" style="48" customWidth="1"/>
     <col min="10" max="10" width="22.5703125" style="46" customWidth="1"/>
@@ -2060,12 +2061,12 @@
     <col min="24" max="24" width="8.5703125" style="59" customWidth="1"/>
     <col min="25" max="25" width="47.7109375" style="11" bestFit="1" customWidth="1"/>
     <col min="26" max="26" width="14.85546875" style="6" customWidth="1"/>
-    <col min="27" max="27" width="11.5703125" style="72" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="11.5703125" style="65" bestFit="1" customWidth="1"/>
     <col min="28" max="28" width="9.140625" style="11"/>
     <col min="29" max="29" width="9.140625" style="9"/>
     <col min="30" max="30" width="40.85546875" style="11" bestFit="1" customWidth="1"/>
     <col min="31" max="31" width="14.85546875" style="9" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="12.42578125" style="70" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="12.42578125" style="64" bestFit="1" customWidth="1"/>
     <col min="33" max="16384" width="9.140625" style="11"/>
   </cols>
   <sheetData>
@@ -2088,7 +2089,7 @@
       <c r="F1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="G1" s="78" t="s">
+      <c r="G1" s="70" t="s">
         <v>4</v>
       </c>
       <c r="H1" s="1" t="s">
@@ -2134,7 +2135,7 @@
       <c r="F2" s="8" t="s">
         <v>71</v>
       </c>
-      <c r="G2" s="72">
+      <c r="G2" s="65">
         <v>6.6666666666666666E-2</v>
       </c>
       <c r="H2" s="6" t="s">
@@ -2183,7 +2184,7 @@
       <c r="F3" s="9">
         <v>8</v>
       </c>
-      <c r="G3" s="72">
+      <c r="G3" s="65">
         <v>5.6250000000000001E-2</v>
       </c>
       <c r="H3" s="6" t="s">
@@ -2232,7 +2233,7 @@
       <c r="F4" s="9">
         <v>7</v>
       </c>
-      <c r="G4" s="72">
+      <c r="G4" s="65">
         <v>4.8611111111111112E-2</v>
       </c>
       <c r="H4" s="6" t="s">
@@ -2266,7 +2267,7 @@
       <c r="S4" s="36"/>
       <c r="T4" s="36"/>
       <c r="U4" s="36"/>
-      <c r="V4" s="76"/>
+      <c r="V4" s="68"/>
     </row>
     <row r="5" spans="1:32" ht="19.5" x14ac:dyDescent="0.3">
       <c r="A5" s="6">
@@ -2288,7 +2289,7 @@
       <c r="F5" s="9">
         <v>8</v>
       </c>
-      <c r="G5" s="72">
+      <c r="G5" s="65">
         <v>5.486111111111111E-2</v>
       </c>
       <c r="H5" s="6" t="s">
@@ -2357,7 +2358,7 @@
       <c r="AE5" s="60" t="s">
         <v>82</v>
       </c>
-      <c r="AF5" s="69" t="s">
+      <c r="AF5" s="63" t="s">
         <v>4</v>
       </c>
     </row>
@@ -2381,7 +2382,7 @@
       <c r="F6" s="9">
         <v>9</v>
       </c>
-      <c r="G6" s="72">
+      <c r="G6" s="65">
         <v>7.7777777777777779E-2</v>
       </c>
       <c r="H6" s="6" t="s">
@@ -2427,7 +2428,7 @@
       <c r="U6" s="6" t="str">
         <v>ASSISTIDO</v>
       </c>
-      <c r="V6" s="73">
+      <c r="V6" s="66">
         <v>6.6666666666666666E-2</v>
       </c>
       <c r="W6" s="41"/>
@@ -2441,7 +2442,7 @@
       <c r="Z6" s="6" t="str">
         <v>ASSISTIDO</v>
       </c>
-      <c r="AA6" s="73">
+      <c r="AA6" s="66">
         <v>4.8611111111111112E-2</v>
       </c>
       <c r="AB6" s="14"/>
@@ -2455,7 +2456,7 @@
       <c r="AE6" s="9" t="str">
         <v>ASSISTIDO</v>
       </c>
-      <c r="AF6" s="70">
+      <c r="AF6" s="64">
         <v>6.805555555555555E-2</v>
       </c>
     </row>
@@ -2479,7 +2480,7 @@
       <c r="F7" s="9" t="s">
         <v>72</v>
       </c>
-      <c r="G7" s="72">
+      <c r="G7" s="65">
         <v>7.4999999999999997E-2</v>
       </c>
       <c r="H7" s="6" t="s">
@@ -2525,7 +2526,7 @@
       <c r="U7" s="6" t="str">
         <v>ASSISTIDO</v>
       </c>
-      <c r="V7" s="73">
+      <c r="V7" s="66">
         <v>5.6250000000000001E-2</v>
       </c>
       <c r="W7" s="41"/>
@@ -2538,7 +2539,7 @@
       <c r="Z7" s="6" t="str">
         <v>ASSISTIDO</v>
       </c>
-      <c r="AA7" s="73">
+      <c r="AA7" s="66">
         <v>5.486111111111111E-2</v>
       </c>
       <c r="AB7" s="14"/>
@@ -2551,7 +2552,7 @@
       <c r="AE7" s="9" t="str">
         <v>ASSISTIDO</v>
       </c>
-      <c r="AF7" s="70">
+      <c r="AF7" s="64">
         <v>7.2916666666666671E-2</v>
       </c>
     </row>
@@ -2575,7 +2576,7 @@
       <c r="F8" s="9">
         <v>9</v>
       </c>
-      <c r="G8" s="72">
+      <c r="G8" s="65">
         <v>6.9444444444444434E-2</v>
       </c>
       <c r="H8" s="6" t="s">
@@ -2621,7 +2622,7 @@
       <c r="U8" s="6" t="str">
         <v>ASSISTIDO</v>
       </c>
-      <c r="V8" s="73">
+      <c r="V8" s="66">
         <v>8.7500000000000008E-2</v>
       </c>
       <c r="W8" s="41"/>
@@ -2634,7 +2635,7 @@
       <c r="Z8" s="6" t="str">
         <v>ASSISTIDO</v>
       </c>
-      <c r="AA8" s="73">
+      <c r="AA8" s="66">
         <v>7.7777777777777779E-2</v>
       </c>
       <c r="AB8" s="14"/>
@@ -2647,7 +2648,7 @@
       <c r="AE8" s="9" t="str">
         <v>ASSISTIDO</v>
       </c>
-      <c r="AF8" s="70">
+      <c r="AF8" s="64">
         <v>7.2222222222222229E-2</v>
       </c>
     </row>
@@ -2671,7 +2672,7 @@
       <c r="F9" s="9" t="s">
         <v>71</v>
       </c>
-      <c r="G9" s="72">
+      <c r="G9" s="65">
         <v>5.9027777777777783E-2</v>
       </c>
       <c r="H9" s="6" t="s">
@@ -2717,7 +2718,7 @@
       <c r="U9" s="6" t="str">
         <v>ASSISTIDO</v>
       </c>
-      <c r="V9" s="73">
+      <c r="V9" s="66">
         <v>6.5972222222222224E-2</v>
       </c>
       <c r="W9" s="41"/>
@@ -2730,7 +2731,7 @@
       <c r="Z9" s="6" t="str">
         <v>ASSISTIDO</v>
       </c>
-      <c r="AA9" s="73">
+      <c r="AA9" s="66">
         <v>7.4999999999999997E-2</v>
       </c>
       <c r="AB9" s="14"/>
@@ -2743,7 +2744,7 @@
       <c r="AE9" s="9" t="str">
         <v>ASSISTIDO</v>
       </c>
-      <c r="AF9" s="70">
+      <c r="AF9" s="64">
         <v>6.1805555555555558E-2</v>
       </c>
     </row>
@@ -2767,7 +2768,7 @@
       <c r="F10" s="9">
         <v>8</v>
       </c>
-      <c r="G10" s="72">
+      <c r="G10" s="65">
         <v>5.7638888888888885E-2</v>
       </c>
       <c r="H10" s="6" t="s">
@@ -2813,7 +2814,7 @@
       <c r="U10" s="6" t="str">
         <v>ASSISTIDO</v>
       </c>
-      <c r="V10" s="73">
+      <c r="V10" s="66">
         <v>7.2916666666666671E-2</v>
       </c>
       <c r="W10" s="41"/>
@@ -2826,7 +2827,7 @@
       <c r="Z10" s="6" t="str">
         <v>ASSISTIDO</v>
       </c>
-      <c r="AA10" s="73">
+      <c r="AA10" s="66">
         <v>5.9027777777777783E-2</v>
       </c>
       <c r="AB10" s="14"/>
@@ -2839,7 +2840,7 @@
       <c r="AE10" s="9" t="str">
         <v>ASSISTIDO</v>
       </c>
-      <c r="AF10" s="70">
+      <c r="AF10" s="64">
         <v>7.2916666666666671E-2</v>
       </c>
     </row>
@@ -2863,7 +2864,7 @@
       <c r="F11" s="9">
         <v>8</v>
       </c>
-      <c r="G11" s="72">
+      <c r="G11" s="65">
         <v>7.2222222222222229E-2</v>
       </c>
       <c r="H11" s="6" t="s">
@@ -2897,7 +2898,7 @@
       </c>
       <c r="Q11" s="31">
         <f>VLOOKUP($Q$6,$A$2:$F$141,6,1)</f>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="R11" s="35"/>
       <c r="S11" s="40">
@@ -2909,7 +2910,7 @@
       <c r="U11" s="6" t="str">
         <v>ASSISTIDO</v>
       </c>
-      <c r="V11" s="73">
+      <c r="V11" s="66">
         <v>6.3888888888888884E-2</v>
       </c>
       <c r="W11" s="41"/>
@@ -2922,7 +2923,7 @@
       <c r="Z11" s="6" t="str">
         <v>ASSISTIDO</v>
       </c>
-      <c r="AA11" s="73">
+      <c r="AA11" s="66">
         <v>5.7638888888888885E-2</v>
       </c>
       <c r="AB11" s="14"/>
@@ -2935,7 +2936,7 @@
       <c r="AE11" s="9" t="str">
         <v>ASSISTIDO</v>
       </c>
-      <c r="AF11" s="70">
+      <c r="AF11" s="64">
         <v>6.458333333333334E-2</v>
       </c>
     </row>
@@ -2959,7 +2960,7 @@
       <c r="F12" s="9">
         <v>10</v>
       </c>
-      <c r="G12" s="72">
+      <c r="G12" s="65">
         <v>7.5694444444444439E-2</v>
       </c>
       <c r="H12" s="6" t="s">
@@ -2993,7 +2994,7 @@
       </c>
       <c r="Q12" s="33" t="str">
         <f>VLOOKUP($Q$6,$A$2:$M$141,13,1)</f>
-        <v>NÃO ASSISTIDO</v>
+        <v>ASSISTIDO</v>
       </c>
       <c r="R12" s="35"/>
       <c r="S12" s="40">
@@ -3005,7 +3006,7 @@
       <c r="U12" s="6" t="str">
         <v>ASSISTIDO</v>
       </c>
-      <c r="V12" s="73">
+      <c r="V12" s="66">
         <v>6.5972222222222224E-2</v>
       </c>
       <c r="W12" s="41"/>
@@ -3018,7 +3019,7 @@
       <c r="Z12" s="6" t="str">
         <v>ASSISTIDO</v>
       </c>
-      <c r="AA12" s="73">
+      <c r="AA12" s="66">
         <v>7.2222222222222229E-2</v>
       </c>
       <c r="AB12" s="14"/>
@@ -3031,7 +3032,7 @@
       <c r="AE12" s="9" t="str">
         <v>ASSISTIDO</v>
       </c>
-      <c r="AF12" s="70">
+      <c r="AF12" s="64">
         <v>5.8333333333333327E-2</v>
       </c>
     </row>
@@ -3055,7 +3056,7 @@
       <c r="F13" s="9">
         <v>9</v>
       </c>
-      <c r="G13" s="72">
+      <c r="G13" s="65">
         <v>6.9444444444444434E-2</v>
       </c>
       <c r="H13" s="6" t="s">
@@ -3096,7 +3097,7 @@
       <c r="U13" s="6" t="str">
         <v>ASSISTIDO</v>
       </c>
-      <c r="V13" s="73">
+      <c r="V13" s="66">
         <v>6.9444444444444434E-2</v>
       </c>
       <c r="W13" s="41"/>
@@ -3109,7 +3110,7 @@
       <c r="Z13" s="6" t="str">
         <v>ASSISTIDO</v>
       </c>
-      <c r="AA13" s="73">
+      <c r="AA13" s="66">
         <v>7.5694444444444439E-2</v>
       </c>
       <c r="AB13" s="14"/>
@@ -3122,7 +3123,7 @@
       <c r="AE13" s="9" t="str">
         <v>ASSISTIDO</v>
       </c>
-      <c r="AF13" s="70">
+      <c r="AF13" s="64">
         <v>6.1805555555555558E-2</v>
       </c>
     </row>
@@ -3146,7 +3147,7 @@
       <c r="F14" s="9">
         <v>9</v>
       </c>
-      <c r="G14" s="72">
+      <c r="G14" s="65">
         <v>7.4305555555555555E-2</v>
       </c>
       <c r="H14" s="6" t="s">
@@ -3189,7 +3190,7 @@
       <c r="U14" s="6" t="str">
         <v>ASSISTIDO</v>
       </c>
-      <c r="V14" s="73">
+      <c r="V14" s="66">
         <v>6.5972222222222224E-2</v>
       </c>
       <c r="W14" s="41"/>
@@ -3202,7 +3203,7 @@
       <c r="Z14" s="6" t="str">
         <v>ASSISTIDO</v>
       </c>
-      <c r="AA14" s="73">
+      <c r="AA14" s="66">
         <v>6.9444444444444434E-2</v>
       </c>
       <c r="AB14" s="14"/>
@@ -3215,7 +3216,7 @@
       <c r="AE14" s="9" t="str">
         <v>ASSISTIDO</v>
       </c>
-      <c r="AF14" s="70">
+      <c r="AF14" s="64">
         <v>6.3888888888888884E-2</v>
       </c>
     </row>
@@ -3239,7 +3240,7 @@
       <c r="F15" s="9">
         <v>9</v>
       </c>
-      <c r="G15" s="72">
+      <c r="G15" s="65">
         <v>7.4999999999999997E-2</v>
       </c>
       <c r="H15" s="6" t="s">
@@ -3272,7 +3273,7 @@
         <v>173</v>
       </c>
       <c r="Q15" s="31" t="s">
-        <v>153</v>
+        <v>89</v>
       </c>
       <c r="R15" s="35"/>
       <c r="S15" s="40">
@@ -3284,7 +3285,7 @@
       <c r="U15" s="6" t="str">
         <v>ASSISTIDO</v>
       </c>
-      <c r="V15" s="73">
+      <c r="V15" s="66">
         <v>7.1527777777777787E-2</v>
       </c>
       <c r="W15" s="41"/>
@@ -3297,7 +3298,7 @@
       <c r="Z15" s="6" t="str">
         <v>ASSISTIDO</v>
       </c>
-      <c r="AA15" s="73">
+      <c r="AA15" s="66">
         <v>7.4305555555555555E-2</v>
       </c>
       <c r="AB15" s="14"/>
@@ -3310,7 +3311,7 @@
       <c r="AE15" s="9" t="str">
         <v>ASSISTIDO</v>
       </c>
-      <c r="AF15" s="70">
+      <c r="AF15" s="64">
         <v>6.3888888888888884E-2</v>
       </c>
     </row>
@@ -3334,7 +3335,7 @@
       <c r="F16" s="9">
         <v>9</v>
       </c>
-      <c r="G16" s="72">
+      <c r="G16" s="65">
         <v>7.9861111111111105E-2</v>
       </c>
       <c r="H16" s="6" t="s">
@@ -3368,7 +3369,7 @@
       </c>
       <c r="Q16" s="31">
         <f>VLOOKUP($Q$15,$B:$N,2,0)</f>
-        <v>1941</v>
+        <v>1950</v>
       </c>
       <c r="R16" s="35"/>
       <c r="S16" s="40">
@@ -3380,7 +3381,7 @@
       <c r="U16" s="6" t="str">
         <v>ASSISTIDO</v>
       </c>
-      <c r="V16" s="73">
+      <c r="V16" s="66">
         <v>6.6666666666666666E-2</v>
       </c>
       <c r="W16" s="41"/>
@@ -3393,7 +3394,7 @@
       <c r="Z16" s="6" t="str">
         <v>ASSISTIDO</v>
       </c>
-      <c r="AA16" s="73">
+      <c r="AA16" s="66">
         <v>7.4999999999999997E-2</v>
       </c>
       <c r="AB16" s="14"/>
@@ -3406,7 +3407,7 @@
       <c r="AE16" s="9" t="str">
         <v>ASSISTIDO</v>
       </c>
-      <c r="AF16" s="70">
+      <c r="AF16" s="64">
         <v>6.5972222222222224E-2</v>
       </c>
     </row>
@@ -3430,7 +3431,7 @@
       <c r="F17" s="9">
         <v>9</v>
       </c>
-      <c r="G17" s="72">
+      <c r="G17" s="65">
         <v>7.4999999999999997E-2</v>
       </c>
       <c r="H17" s="6" t="s">
@@ -3476,7 +3477,7 @@
       <c r="U17" s="6" t="str">
         <v>ASSISTIDO</v>
       </c>
-      <c r="V17" s="73">
+      <c r="V17" s="66">
         <v>7.2222222222222229E-2</v>
       </c>
       <c r="W17" s="41"/>
@@ -3489,7 +3490,7 @@
       <c r="Z17" s="6" t="str">
         <v>ASSISTIDO</v>
       </c>
-      <c r="AA17" s="73">
+      <c r="AA17" s="66">
         <v>7.9861111111111105E-2</v>
       </c>
       <c r="AB17" s="14"/>
@@ -3502,7 +3503,7 @@
       <c r="AE17" s="9" t="str">
         <v>ASSISTIDO</v>
       </c>
-      <c r="AF17" s="70">
+      <c r="AF17" s="64">
         <v>6.7361111111111108E-2</v>
       </c>
     </row>
@@ -3526,7 +3527,7 @@
       <c r="F18" s="9" t="s">
         <v>71</v>
       </c>
-      <c r="G18" s="72">
+      <c r="G18" s="65">
         <v>5.9027777777777783E-2</v>
       </c>
       <c r="H18" s="6" t="s">
@@ -3560,7 +3561,7 @@
       </c>
       <c r="Q18" s="50">
         <f>VLOOKUP($Q$15,$B:$N,6,0)</f>
-        <v>4.4444444444444446E-2</v>
+        <v>5.1388888888888894E-2</v>
       </c>
       <c r="R18" s="35"/>
       <c r="S18" s="40">
@@ -3572,7 +3573,7 @@
       <c r="U18" s="6" t="str">
         <v>ASSISTIDO</v>
       </c>
-      <c r="V18" s="73">
+      <c r="V18" s="66">
         <v>6.805555555555555E-2</v>
       </c>
       <c r="W18" s="41"/>
@@ -3585,7 +3586,7 @@
       <c r="Z18" s="6" t="str">
         <v>ASSISTIDO</v>
       </c>
-      <c r="AA18" s="73">
+      <c r="AA18" s="66">
         <v>7.4999999999999997E-2</v>
       </c>
       <c r="AB18" s="14"/>
@@ -3598,7 +3599,7 @@
       <c r="AE18" s="9" t="str">
         <v>ASSISTIDO</v>
       </c>
-      <c r="AF18" s="70">
+      <c r="AF18" s="64">
         <v>6.25E-2</v>
       </c>
     </row>
@@ -3622,7 +3623,7 @@
       <c r="F19" s="9" t="s">
         <v>71</v>
       </c>
-      <c r="G19" s="72">
+      <c r="G19" s="65">
         <v>8.7500000000000008E-2</v>
       </c>
       <c r="H19" s="6" t="s">
@@ -3668,7 +3669,7 @@
       <c r="U19" s="6" t="str">
         <v>ASSISTIDO</v>
       </c>
-      <c r="V19" s="73">
+      <c r="V19" s="66">
         <v>7.7083333333333337E-2</v>
       </c>
       <c r="W19" s="41"/>
@@ -3681,7 +3682,7 @@
       <c r="Z19" s="6" t="str">
         <v>ASSISTIDO</v>
       </c>
-      <c r="AA19" s="73">
+      <c r="AA19" s="66">
         <v>5.9027777777777783E-2</v>
       </c>
       <c r="AB19" s="14"/>
@@ -3694,7 +3695,7 @@
       <c r="AE19" s="9" t="str">
         <v>ASSISTIDO</v>
       </c>
-      <c r="AF19" s="70">
+      <c r="AF19" s="64">
         <v>5.9722222222222225E-2</v>
       </c>
     </row>
@@ -3718,7 +3719,7 @@
       <c r="F20" s="9">
         <v>10</v>
       </c>
-      <c r="G20" s="72">
+      <c r="G20" s="65">
         <v>6.5972222222222224E-2</v>
       </c>
       <c r="H20" s="6" t="s">
@@ -3764,7 +3765,7 @@
       <c r="U20" s="6" t="str">
         <v>ASSISTIDO</v>
       </c>
-      <c r="V20" s="73">
+      <c r="V20" s="66">
         <v>6.9444444444444434E-2</v>
       </c>
       <c r="W20" s="41"/>
@@ -3777,7 +3778,7 @@
       <c r="Z20" s="6" t="str">
         <v>ASSISTIDO</v>
       </c>
-      <c r="AA20" s="73">
+      <c r="AA20" s="66">
         <v>6.5972222222222224E-2</v>
       </c>
       <c r="AB20" s="14"/>
@@ -3790,7 +3791,7 @@
       <c r="AE20" s="9" t="str">
         <v>ASSISTIDO</v>
       </c>
-      <c r="AF20" s="70">
+      <c r="AF20" s="64">
         <v>7.0833333333333331E-2</v>
       </c>
     </row>
@@ -3814,7 +3815,7 @@
       <c r="F21" s="9">
         <v>9</v>
       </c>
-      <c r="G21" s="72">
+      <c r="G21" s="65">
         <v>7.2916666666666671E-2</v>
       </c>
       <c r="H21" s="6" t="s">
@@ -3847,7 +3848,7 @@
       </c>
       <c r="Q21" s="31">
         <f>VLOOKUP($Q$15,$B:$N,13,0)</f>
-        <v>125</v>
+        <v>105</v>
       </c>
       <c r="R21" s="26"/>
       <c r="S21" s="40">
@@ -3859,7 +3860,7 @@
       <c r="U21" s="6" t="str">
         <v>ASSISTIDO</v>
       </c>
-      <c r="V21" s="73">
+      <c r="V21" s="66">
         <v>6.9444444444444434E-2</v>
       </c>
       <c r="W21" s="41"/>
@@ -3872,7 +3873,7 @@
       <c r="Z21" s="6" t="str">
         <v>ASSISTIDO</v>
       </c>
-      <c r="AA21" s="73">
+      <c r="AA21" s="66">
         <v>5.2777777777777778E-2</v>
       </c>
       <c r="AB21" s="14"/>
@@ -3885,7 +3886,7 @@
       <c r="AE21" s="9" t="str">
         <v>NÃO ASSISTIDO</v>
       </c>
-      <c r="AF21" s="70">
+      <c r="AF21" s="64">
         <v>5.9722222222222225E-2</v>
       </c>
     </row>
@@ -3909,7 +3910,7 @@
       <c r="F22" s="9">
         <v>9</v>
       </c>
-      <c r="G22" s="72">
+      <c r="G22" s="65">
         <v>6.3888888888888884E-2</v>
       </c>
       <c r="H22" s="6" t="s">
@@ -3947,7 +3948,7 @@
       <c r="U22" s="6" t="str">
         <v>ASSISTIDO</v>
       </c>
-      <c r="V22" s="73">
+      <c r="V22" s="66">
         <v>6.458333333333334E-2</v>
       </c>
       <c r="W22" s="41"/>
@@ -3960,7 +3961,7 @@
       <c r="Z22" s="6" t="str">
         <v>ASSISTIDO</v>
       </c>
-      <c r="AA22" s="73">
+      <c r="AA22" s="66">
         <v>5.2083333333333336E-2</v>
       </c>
       <c r="AB22" s="14"/>
@@ -3973,7 +3974,7 @@
       <c r="AE22" s="9" t="str">
         <v>NÃO ASSISTIDO</v>
       </c>
-      <c r="AF22" s="70">
+      <c r="AF22" s="64">
         <v>6.8749999999999992E-2</v>
       </c>
     </row>
@@ -3997,7 +3998,7 @@
       <c r="F23" s="9" t="s">
         <v>71</v>
       </c>
-      <c r="G23" s="72">
+      <c r="G23" s="65">
         <v>6.805555555555555E-2</v>
       </c>
       <c r="H23" s="6" t="s">
@@ -4039,7 +4040,7 @@
       <c r="U23" s="6" t="str">
         <v>ASSISTIDO</v>
       </c>
-      <c r="V23" s="73">
+      <c r="V23" s="66">
         <v>8.1250000000000003E-2</v>
       </c>
       <c r="W23" s="41"/>
@@ -4052,7 +4053,7 @@
       <c r="Z23" s="6" t="str">
         <v>ASSISTIDO</v>
       </c>
-      <c r="AA23" s="73">
+      <c r="AA23" s="66">
         <v>7.0833333333333331E-2</v>
       </c>
       <c r="AB23" s="14"/>
@@ -4065,7 +4066,7 @@
       <c r="AE23" s="9" t="str">
         <v>NÃO ASSISTIDO</v>
       </c>
-      <c r="AF23" s="70">
+      <c r="AF23" s="64">
         <v>5.7638888888888885E-2</v>
       </c>
     </row>
@@ -4089,7 +4090,7 @@
       <c r="F24" s="9">
         <v>9</v>
       </c>
-      <c r="G24" s="72">
+      <c r="G24" s="65">
         <v>7.2916666666666671E-2</v>
       </c>
       <c r="H24" s="6" t="s">
@@ -4121,7 +4122,7 @@
         <v>5</v>
       </c>
       <c r="Q24" s="19" t="s">
-        <v>84</v>
+        <v>10</v>
       </c>
       <c r="R24" s="26"/>
       <c r="S24" s="40">
@@ -4133,7 +4134,7 @@
       <c r="U24" s="6" t="str">
         <v>ASSISTIDO</v>
       </c>
-      <c r="V24" s="73">
+      <c r="V24" s="66">
         <v>7.3611111111111113E-2</v>
       </c>
       <c r="W24" s="41"/>
@@ -4146,7 +4147,7 @@
       <c r="Z24" s="6" t="str">
         <v>ASSISTIDO</v>
       </c>
-      <c r="AA24" s="73">
+      <c r="AA24" s="66">
         <v>6.1111111111111116E-2</v>
       </c>
       <c r="AB24" s="14"/>
@@ -4159,7 +4160,7 @@
       <c r="AE24" s="9" t="str">
         <v>NÃO ASSISTIDO</v>
       </c>
-      <c r="AF24" s="70">
+      <c r="AF24" s="64">
         <v>6.25E-2</v>
       </c>
     </row>
@@ -4183,7 +4184,7 @@
       <c r="F25" s="9">
         <v>8</v>
       </c>
-      <c r="G25" s="72">
+      <c r="G25" s="65">
         <v>7.2222222222222229E-2</v>
       </c>
       <c r="H25" s="6" t="s">
@@ -4216,7 +4217,7 @@
       </c>
       <c r="Q25" s="20">
         <f>COUNTIF(H:H,$Q$24)</f>
-        <v>10</v>
+        <v>70</v>
       </c>
       <c r="R25" s="26"/>
       <c r="S25" s="40">
@@ -4228,7 +4229,7 @@
       <c r="U25" s="6" t="str">
         <v>ASSISTIDO</v>
       </c>
-      <c r="V25" s="73">
+      <c r="V25" s="66">
         <v>7.5694444444444439E-2</v>
       </c>
       <c r="W25" s="41"/>
@@ -4241,7 +4242,7 @@
       <c r="Z25" s="6" t="str">
         <v>ASSISTIDO</v>
       </c>
-      <c r="AA25" s="73">
+      <c r="AA25" s="66">
         <v>6.0416666666666667E-2</v>
       </c>
       <c r="AB25" s="14"/>
@@ -4254,7 +4255,7 @@
       <c r="AE25" s="9" t="str">
         <v>ASSISTIDO</v>
       </c>
-      <c r="AF25" s="70">
+      <c r="AF25" s="64">
         <v>5.9027777777777783E-2</v>
       </c>
     </row>
@@ -4278,7 +4279,7 @@
       <c r="F26" s="9" t="s">
         <v>71</v>
       </c>
-      <c r="G26" s="72">
+      <c r="G26" s="65">
         <v>6.1805555555555558E-2</v>
       </c>
       <c r="H26" s="6" t="s">
@@ -4311,7 +4312,7 @@
       </c>
       <c r="Q26" s="22">
         <f>SUMIF(H:H,$Q$24,L:L)</f>
-        <v>7</v>
+        <v>46</v>
       </c>
       <c r="R26" s="26"/>
       <c r="S26" s="40">
@@ -4323,7 +4324,7 @@
       <c r="U26" s="6" t="str">
         <v>NÃO ASSISTIDO</v>
       </c>
-      <c r="V26" s="73">
+      <c r="V26" s="66">
         <v>6.458333333333334E-2</v>
       </c>
       <c r="W26" s="41"/>
@@ -4336,7 +4337,7 @@
       <c r="Z26" s="6" t="str">
         <v>ASSISTIDO</v>
       </c>
-      <c r="AA26" s="73">
+      <c r="AA26" s="66">
         <v>5.6250000000000001E-2</v>
       </c>
       <c r="AB26" s="14"/>
@@ -4349,7 +4350,7 @@
       <c r="AE26" s="9" t="str">
         <v>NÃO ASSISTIDO</v>
       </c>
-      <c r="AF26" s="70">
+      <c r="AF26" s="64">
         <v>6.0416666666666667E-2</v>
       </c>
     </row>
@@ -4373,7 +4374,7 @@
       <c r="F27" s="9" t="s">
         <v>72</v>
       </c>
-      <c r="G27" s="72">
+      <c r="G27" s="65">
         <v>7.2916666666666671E-2</v>
       </c>
       <c r="H27" s="6" t="s">
@@ -4406,7 +4407,7 @@
       </c>
       <c r="Q27" s="21">
         <f>$Q$25-$Q$26</f>
-        <v>3</v>
+        <v>24</v>
       </c>
       <c r="R27" s="26"/>
       <c r="S27" s="40">
@@ -4418,7 +4419,7 @@
       <c r="U27" s="6" t="str">
         <v>ASSISTIDO</v>
       </c>
-      <c r="V27" s="73">
+      <c r="V27" s="66">
         <v>6.6666666666666666E-2</v>
       </c>
       <c r="W27" s="41"/>
@@ -4431,7 +4432,7 @@
       <c r="Z27" s="6" t="str">
         <v>ASSISTIDO</v>
       </c>
-      <c r="AA27" s="73">
+      <c r="AA27" s="66">
         <v>6.25E-2</v>
       </c>
       <c r="AB27" s="14"/>
@@ -4444,7 +4445,7 @@
       <c r="AE27" s="9" t="str">
         <v>NÃO ASSISTIDO</v>
       </c>
-      <c r="AF27" s="70">
+      <c r="AF27" s="64">
         <v>5.9722222222222225E-2</v>
       </c>
     </row>
@@ -4468,7 +4469,7 @@
       <c r="F28" s="9">
         <v>8</v>
       </c>
-      <c r="G28" s="72">
+      <c r="G28" s="65">
         <v>6.458333333333334E-2</v>
       </c>
       <c r="H28" s="6" t="s">
@@ -4506,7 +4507,7 @@
       <c r="U28" s="11" t="str">
         <v>ASSISTIDO</v>
       </c>
-      <c r="V28" s="73">
+      <c r="V28" s="66">
         <v>7.0833333333333331E-2</v>
       </c>
       <c r="W28" s="41"/>
@@ -4519,7 +4520,7 @@
       <c r="Z28" s="6" t="str">
         <v>ASSISTIDO</v>
       </c>
-      <c r="AA28" s="73">
+      <c r="AA28" s="66">
         <v>6.458333333333334E-2</v>
       </c>
       <c r="AB28" s="14"/>
@@ -4532,7 +4533,7 @@
       <c r="AE28" s="9" t="str">
         <v>NÃO ASSISTIDO</v>
       </c>
-      <c r="AF28" s="70">
+      <c r="AF28" s="64">
         <v>6.3194444444444442E-2</v>
       </c>
     </row>
@@ -4556,7 +4557,7 @@
       <c r="F29" s="9" t="s">
         <v>71</v>
       </c>
-      <c r="G29" s="72">
+      <c r="G29" s="65">
         <v>5.8333333333333327E-2</v>
       </c>
       <c r="H29" s="6" t="s">
@@ -4598,7 +4599,7 @@
       <c r="U29" s="11" t="str">
         <v>NÃO ASSISTIDO</v>
       </c>
-      <c r="V29" s="73">
+      <c r="V29" s="66">
         <v>7.2916666666666671E-2</v>
       </c>
       <c r="W29" s="41"/>
@@ -4611,7 +4612,7 @@
       <c r="Z29" s="6" t="str">
         <v>ASSISTIDO</v>
       </c>
-      <c r="AA29" s="73">
+      <c r="AA29" s="66">
         <v>5.8333333333333327E-2</v>
       </c>
       <c r="AB29" s="14"/>
@@ -4624,7 +4625,7 @@
       <c r="AE29" s="9" t="str">
         <v>ASSISTIDO</v>
       </c>
-      <c r="AF29" s="70">
+      <c r="AF29" s="64">
         <v>6.1805555555555558E-2</v>
       </c>
     </row>
@@ -4648,7 +4649,7 @@
       <c r="F30" s="9" t="s">
         <v>73</v>
       </c>
-      <c r="G30" s="72">
+      <c r="G30" s="65">
         <v>6.1805555555555558E-2</v>
       </c>
       <c r="H30" s="6" t="s">
@@ -4681,7 +4682,7 @@
       </c>
       <c r="Q30" s="19">
         <f>COUNTIF(M:M,"ASSISTIDO")</f>
-        <v>146</v>
+        <v>148</v>
       </c>
       <c r="R30" s="26"/>
       <c r="S30" s="40">
@@ -4693,7 +4694,7 @@
       <c r="U30" s="11" t="str">
         <v>NÃO ASSISTIDO</v>
       </c>
-      <c r="V30" s="73">
+      <c r="V30" s="66">
         <v>6.9444444444444434E-2</v>
       </c>
       <c r="W30" s="41"/>
@@ -4706,7 +4707,7 @@
       <c r="Z30" s="6" t="str">
         <v>ASSISTIDO</v>
       </c>
-      <c r="AA30" s="73">
+      <c r="AA30" s="66">
         <v>6.3194444444444442E-2</v>
       </c>
       <c r="AB30" s="14"/>
@@ -4719,7 +4720,7 @@
       <c r="AE30" s="9" t="str">
         <v>NÃO ASSISTIDO</v>
       </c>
-      <c r="AF30" s="70">
+      <c r="AF30" s="64">
         <v>7.0833333333333331E-2</v>
       </c>
     </row>
@@ -4743,7 +4744,7 @@
       <c r="F31" s="9" t="s">
         <v>71</v>
       </c>
-      <c r="G31" s="72">
+      <c r="G31" s="65">
         <v>6.5972222222222224E-2</v>
       </c>
       <c r="H31" s="6" t="s">
@@ -4776,15 +4777,15 @@
       </c>
       <c r="Q31" s="19">
         <f>COUNTIF(M:M,"NÃO ASSISTIDO")</f>
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="R31" s="26"/>
-      <c r="S31" s="63" t="s">
+      <c r="S31" s="71" t="s">
         <v>206</v>
       </c>
-      <c r="T31" s="64"/>
-      <c r="U31" s="65"/>
-      <c r="V31" s="75">
+      <c r="T31" s="72"/>
+      <c r="U31" s="73"/>
+      <c r="V31" s="77">
         <f ca="1">SUMIF($U$6:$V$30,"ASSISTIDO",$V$6:$V$30)</f>
         <v>1.5416666666666667</v>
       </c>
@@ -4798,7 +4799,7 @@
       <c r="Z31" s="6" t="str">
         <v>ASSISTIDO</v>
       </c>
-      <c r="AA31" s="73">
+      <c r="AA31" s="66">
         <v>6.1805555555555558E-2</v>
       </c>
       <c r="AB31" s="14"/>
@@ -4811,7 +4812,7 @@
       <c r="AE31" s="9" t="str">
         <v>NÃO ASSISTIDO</v>
       </c>
-      <c r="AF31" s="70">
+      <c r="AF31" s="64">
         <v>6.458333333333334E-2</v>
       </c>
     </row>
@@ -4835,7 +4836,7 @@
       <c r="F32" s="9">
         <v>9</v>
       </c>
-      <c r="G32" s="72">
+      <c r="G32" s="65">
         <v>6.5972222222222224E-2</v>
       </c>
       <c r="H32" s="6" t="s">
@@ -4873,7 +4874,7 @@
       <c r="S32" s="37"/>
       <c r="T32" s="37"/>
       <c r="U32" s="37"/>
-      <c r="V32" s="77"/>
+      <c r="V32" s="69"/>
       <c r="W32" s="42"/>
       <c r="X32" s="62">
         <v>48</v>
@@ -4884,7 +4885,7 @@
       <c r="Z32" s="6" t="str">
         <v>ASSISTIDO</v>
       </c>
-      <c r="AA32" s="73">
+      <c r="AA32" s="66">
         <v>5.7638888888888885E-2</v>
       </c>
       <c r="AB32" s="14"/>
@@ -4897,7 +4898,7 @@
       <c r="AE32" s="9" t="str">
         <v>NÃO ASSISTIDO</v>
       </c>
-      <c r="AF32" s="70">
+      <c r="AF32" s="64">
         <v>6.6666666666666666E-2</v>
       </c>
     </row>
@@ -4921,7 +4922,7 @@
       <c r="F33" s="9">
         <v>8</v>
       </c>
-      <c r="G33" s="72">
+      <c r="G33" s="65">
         <v>5.2777777777777778E-2</v>
       </c>
       <c r="H33" s="6" t="s">
@@ -4959,7 +4960,7 @@
       <c r="Z33" s="6" t="str">
         <v>ASSISTIDO</v>
       </c>
-      <c r="AA33" s="73">
+      <c r="AA33" s="66">
         <v>6.7361111111111108E-2</v>
       </c>
       <c r="AB33" s="14"/>
@@ -4970,9 +4971,9 @@
         <v>Madagascar 3: Os Procurados</v>
       </c>
       <c r="AE33" s="9" t="str">
-        <v>NÃO ASSISTIDO</v>
-      </c>
-      <c r="AF33" s="70">
+        <v>ASSISTIDO</v>
+      </c>
+      <c r="AF33" s="64">
         <v>6.5972222222222224E-2</v>
       </c>
     </row>
@@ -4996,7 +4997,7 @@
       <c r="F34" s="9">
         <v>9</v>
       </c>
-      <c r="G34" s="72">
+      <c r="G34" s="65">
         <v>6.3888888888888884E-2</v>
       </c>
       <c r="H34" s="6" t="s">
@@ -5034,7 +5035,7 @@
       <c r="Z34" s="6" t="str">
         <v>ASSISTIDO</v>
       </c>
-      <c r="AA34" s="73">
+      <c r="AA34" s="66">
         <v>6.1111111111111116E-2</v>
       </c>
       <c r="AB34" s="14"/>
@@ -5047,7 +5048,7 @@
       <c r="AE34" s="9" t="str">
         <v>NÃO ASSISTIDO</v>
       </c>
-      <c r="AF34" s="70">
+      <c r="AF34" s="64">
         <v>6.6666666666666666E-2</v>
       </c>
     </row>
@@ -5071,7 +5072,7 @@
       <c r="F35" s="9" t="s">
         <v>71</v>
       </c>
-      <c r="G35" s="72">
+      <c r="G35" s="65">
         <v>6.3888888888888884E-2</v>
       </c>
       <c r="H35" s="6" t="s">
@@ -5109,7 +5110,7 @@
       <c r="Z35" s="6" t="str">
         <v>ASSISTIDO</v>
       </c>
-      <c r="AA35" s="73">
+      <c r="AA35" s="66">
         <v>9.930555555555555E-2</v>
       </c>
       <c r="AB35" s="14"/>
@@ -5122,7 +5123,7 @@
       <c r="AE35" s="9" t="str">
         <v>NÃO ASSISTIDO</v>
       </c>
-      <c r="AF35" s="70">
+      <c r="AF35" s="64">
         <v>6.3888888888888884E-2</v>
       </c>
     </row>
@@ -5146,7 +5147,7 @@
       <c r="F36" s="9" t="s">
         <v>71</v>
       </c>
-      <c r="G36" s="72">
+      <c r="G36" s="65">
         <v>6.5972222222222224E-2</v>
       </c>
       <c r="H36" s="6" t="s">
@@ -5184,7 +5185,7 @@
       <c r="Z36" s="6" t="str">
         <v>ASSISTIDO</v>
       </c>
-      <c r="AA36" s="73">
+      <c r="AA36" s="66">
         <v>0.10486111111111111</v>
       </c>
       <c r="AB36" s="14"/>
@@ -5197,7 +5198,7 @@
       <c r="AE36" s="9" t="str">
         <v>NÃO ASSISTIDO</v>
       </c>
-      <c r="AF36" s="70">
+      <c r="AF36" s="64">
         <v>6.3888888888888884E-2</v>
       </c>
     </row>
@@ -5221,7 +5222,7 @@
       <c r="F37" s="9" t="s">
         <v>71</v>
       </c>
-      <c r="G37" s="72">
+      <c r="G37" s="65">
         <v>6.7361111111111108E-2</v>
       </c>
       <c r="H37" s="6" t="s">
@@ -5259,7 +5260,7 @@
       <c r="Z37" s="6" t="str">
         <v>ASSISTIDO</v>
       </c>
-      <c r="AA37" s="73">
+      <c r="AA37" s="66">
         <v>0.11666666666666665</v>
       </c>
       <c r="AB37" s="14"/>
@@ -5272,7 +5273,7 @@
       <c r="AE37" s="9" t="str">
         <v>NÃO ASSISTIDO</v>
       </c>
-      <c r="AF37" s="70">
+      <c r="AF37" s="64">
         <v>6.5277777777777782E-2</v>
       </c>
     </row>
@@ -5296,7 +5297,7 @@
       <c r="F38" s="9">
         <v>8</v>
       </c>
-      <c r="G38" s="72">
+      <c r="G38" s="65">
         <v>6.25E-2</v>
       </c>
       <c r="H38" s="6" t="s">
@@ -5334,7 +5335,7 @@
       <c r="Z38" s="6" t="str">
         <v>ASSISTIDO</v>
       </c>
-      <c r="AA38" s="73">
+      <c r="AA38" s="66">
         <v>9.7916666666666666E-2</v>
       </c>
       <c r="AB38" s="14"/>
@@ -5347,7 +5348,7 @@
       <c r="AE38" s="9" t="str">
         <v>NÃO ASSISTIDO</v>
       </c>
-      <c r="AF38" s="70">
+      <c r="AF38" s="64">
         <v>6.458333333333334E-2</v>
       </c>
     </row>
@@ -5371,7 +5372,7 @@
       <c r="F39" s="9">
         <v>8</v>
       </c>
-      <c r="G39" s="72">
+      <c r="G39" s="65">
         <v>5.2083333333333336E-2</v>
       </c>
       <c r="H39" s="6" t="s">
@@ -5409,7 +5410,7 @@
       <c r="Z39" s="6" t="str">
         <v>ASSISTIDO</v>
       </c>
-      <c r="AA39" s="73">
+      <c r="AA39" s="66">
         <v>8.9583333333333334E-2</v>
       </c>
       <c r="AB39" s="14"/>
@@ -5422,7 +5423,7 @@
       <c r="AE39" s="9" t="str">
         <v>NÃO ASSISTIDO</v>
       </c>
-      <c r="AF39" s="70">
+      <c r="AF39" s="64">
         <v>6.7361111111111108E-2</v>
       </c>
     </row>
@@ -5446,7 +5447,7 @@
       <c r="F40" s="9">
         <v>9</v>
       </c>
-      <c r="G40" s="72">
+      <c r="G40" s="65">
         <v>7.0833333333333331E-2</v>
       </c>
       <c r="H40" s="6" t="s">
@@ -5484,7 +5485,7 @@
       <c r="Z40" s="6" t="str">
         <v>ASSISTIDO</v>
       </c>
-      <c r="AA40" s="73">
+      <c r="AA40" s="66">
         <v>5.6250000000000001E-2</v>
       </c>
       <c r="AB40" s="14"/>
@@ -5497,7 +5498,7 @@
       <c r="AE40" s="9" t="str">
         <v>NÃO ASSISTIDO</v>
       </c>
-      <c r="AF40" s="70">
+      <c r="AF40" s="64">
         <v>6.1805555555555558E-2</v>
       </c>
     </row>
@@ -5521,7 +5522,7 @@
       <c r="F41" s="9">
         <v>9</v>
       </c>
-      <c r="G41" s="72">
+      <c r="G41" s="65">
         <v>6.1111111111111116E-2</v>
       </c>
       <c r="H41" s="6" t="s">
@@ -5559,7 +5560,7 @@
       <c r="Z41" s="6" t="str">
         <v>ASSISTIDO</v>
       </c>
-      <c r="AA41" s="73">
+      <c r="AA41" s="66">
         <v>5.1388888888888894E-2</v>
       </c>
       <c r="AB41" s="14"/>
@@ -5572,7 +5573,7 @@
       <c r="AE41" s="9" t="str">
         <v>NÃO ASSISTIDO</v>
       </c>
-      <c r="AF41" s="70">
+      <c r="AF41" s="64">
         <v>6.3888888888888884E-2</v>
       </c>
     </row>
@@ -5596,7 +5597,7 @@
       <c r="F42" s="9" t="s">
         <v>72</v>
       </c>
-      <c r="G42" s="72">
+      <c r="G42" s="65">
         <v>6.0416666666666667E-2</v>
       </c>
       <c r="H42" s="6" t="s">
@@ -5634,7 +5635,7 @@
       <c r="Z42" s="6" t="str">
         <v>ASSISTIDO</v>
       </c>
-      <c r="AA42" s="73">
+      <c r="AA42" s="66">
         <v>5.4166666666666669E-2</v>
       </c>
       <c r="AB42" s="14"/>
@@ -5647,7 +5648,7 @@
       <c r="AE42" s="9" t="str">
         <v>NÃO ASSISTIDO</v>
       </c>
-      <c r="AF42" s="70">
+      <c r="AF42" s="64">
         <v>6.3194444444444442E-2</v>
       </c>
     </row>
@@ -5671,7 +5672,7 @@
       <c r="F43" s="9">
         <v>9</v>
       </c>
-      <c r="G43" s="72">
+      <c r="G43" s="65">
         <v>5.6250000000000001E-2</v>
       </c>
       <c r="H43" s="6" t="s">
@@ -5707,9 +5708,9 @@
         <v>Cinderela</v>
       </c>
       <c r="Z43" s="6" t="str">
-        <v>NÃO ASSISTIDO</v>
-      </c>
-      <c r="AA43" s="73">
+        <v>ASSISTIDO</v>
+      </c>
+      <c r="AA43" s="66">
         <v>5.1388888888888894E-2</v>
       </c>
       <c r="AB43" s="14"/>
@@ -5722,7 +5723,7 @@
       <c r="AE43" s="9" t="str">
         <v>NÃO ASSISTIDO</v>
       </c>
-      <c r="AF43" s="70">
+      <c r="AF43" s="64">
         <v>6.805555555555555E-2</v>
       </c>
     </row>
@@ -5746,7 +5747,7 @@
       <c r="F44" s="9">
         <v>8</v>
       </c>
-      <c r="G44" s="72">
+      <c r="G44" s="65">
         <v>6.25E-2</v>
       </c>
       <c r="H44" s="6" t="s">
@@ -5784,7 +5785,7 @@
       <c r="Z44" s="6" t="str">
         <v>ASSISTIDO</v>
       </c>
-      <c r="AA44" s="73">
+      <c r="AA44" s="66">
         <v>5.2777777777777778E-2</v>
       </c>
       <c r="AB44" s="14"/>
@@ -5797,7 +5798,7 @@
       <c r="AE44" s="9" t="str">
         <v>NÃO ASSISTIDO</v>
       </c>
-      <c r="AF44" s="70">
+      <c r="AF44" s="64">
         <v>6.5972222222222224E-2</v>
       </c>
     </row>
@@ -5821,7 +5822,7 @@
       <c r="F45" s="9" t="s">
         <v>71</v>
       </c>
-      <c r="G45" s="72">
+      <c r="G45" s="65">
         <v>6.458333333333334E-2</v>
       </c>
       <c r="H45" s="6" t="s">
@@ -5859,7 +5860,7 @@
       <c r="Z45" s="6" t="str">
         <v>ASSISTIDO</v>
       </c>
-      <c r="AA45" s="73">
+      <c r="AA45" s="66">
         <v>5.2777777777777778E-2</v>
       </c>
       <c r="AB45" s="14"/>
@@ -5872,7 +5873,7 @@
       <c r="AE45" s="9" t="str">
         <v>NÃO ASSISTIDO</v>
       </c>
-      <c r="AF45" s="70">
+      <c r="AF45" s="64">
         <v>6.1111111111111116E-2</v>
       </c>
     </row>
@@ -5896,7 +5897,7 @@
       <c r="F46" s="9">
         <v>8</v>
       </c>
-      <c r="G46" s="72">
+      <c r="G46" s="65">
         <v>5.8333333333333327E-2</v>
       </c>
       <c r="H46" s="10" t="s">
@@ -5934,7 +5935,7 @@
       <c r="Z46" s="6" t="str">
         <v>ASSISTIDO</v>
       </c>
-      <c r="AA46" s="73">
+      <c r="AA46" s="66">
         <v>5.4166666666666669E-2</v>
       </c>
       <c r="AB46" s="14"/>
@@ -5947,7 +5948,7 @@
       <c r="AE46" s="9" t="str">
         <v>NÃO ASSISTIDO</v>
       </c>
-      <c r="AF46" s="70">
+      <c r="AF46" s="64">
         <v>7.4305555555555555E-2</v>
       </c>
     </row>
@@ -5971,7 +5972,7 @@
       <c r="F47" s="9">
         <v>9</v>
       </c>
-      <c r="G47" s="72">
+      <c r="G47" s="65">
         <v>6.3194444444444442E-2</v>
       </c>
       <c r="H47" s="6" t="s">
@@ -6009,18 +6010,18 @@
       <c r="Z47" s="6" t="str">
         <v>ASSISTIDO</v>
       </c>
-      <c r="AA47" s="73">
+      <c r="AA47" s="66">
         <v>5.4166666666666669E-2</v>
       </c>
       <c r="AB47" s="14"/>
-      <c r="AC47" s="66" t="s">
+      <c r="AC47" s="74" t="s">
         <v>255</v>
       </c>
-      <c r="AD47" s="67"/>
-      <c r="AE47" s="68"/>
-      <c r="AF47" s="71">
+      <c r="AD47" s="75"/>
+      <c r="AE47" s="76"/>
+      <c r="AF47" s="78">
         <f>SUMIF($AE$6:$AE$46,"ASSISTIDO",$AF$6:$AF$46)</f>
-        <v>1.1076388888888888</v>
+        <v>1.1736111111111112</v>
       </c>
     </row>
     <row r="48" spans="1:32" x14ac:dyDescent="0.25">
@@ -6043,7 +6044,7 @@
       <c r="F48" s="9" t="s">
         <v>73</v>
       </c>
-      <c r="G48" s="72">
+      <c r="G48" s="65">
         <v>6.1805555555555558E-2</v>
       </c>
       <c r="H48" s="6" t="s">
@@ -6081,7 +6082,7 @@
       <c r="Z48" s="6" t="str">
         <v>ASSISTIDO</v>
       </c>
-      <c r="AA48" s="73">
+      <c r="AA48" s="66">
         <v>5.6250000000000001E-2</v>
       </c>
       <c r="AB48" s="14"/>
@@ -6106,7 +6107,7 @@
       <c r="F49" s="9" t="s">
         <v>72</v>
       </c>
-      <c r="G49" s="72">
+      <c r="G49" s="65">
         <v>5.7638888888888885E-2</v>
       </c>
       <c r="H49" s="6" t="s">
@@ -6144,7 +6145,7 @@
       <c r="Z49" s="6" t="str">
         <v>NÃO ASSISTIDO</v>
       </c>
-      <c r="AA49" s="73">
+      <c r="AA49" s="66">
         <v>6.5972222222222224E-2</v>
       </c>
       <c r="AB49" s="14"/>
@@ -6169,7 +6170,7 @@
       <c r="F50" s="9">
         <v>8</v>
       </c>
-      <c r="G50" s="72">
+      <c r="G50" s="65">
         <v>6.7361111111111108E-2</v>
       </c>
       <c r="H50" s="6" t="s">
@@ -6207,7 +6208,7 @@
       <c r="Z50" s="6" t="str">
         <v>ASSISTIDO</v>
       </c>
-      <c r="AA50" s="73">
+      <c r="AA50" s="66">
         <v>4.4444444444444446E-2</v>
       </c>
       <c r="AB50" s="14"/>
@@ -6232,7 +6233,7 @@
       <c r="F51" s="9" t="s">
         <v>71</v>
       </c>
-      <c r="G51" s="72">
+      <c r="G51" s="65">
         <v>6.1111111111111116E-2</v>
       </c>
       <c r="H51" s="6" t="s">
@@ -6270,7 +6271,7 @@
       <c r="Z51" s="6" t="str">
         <v>NÃO ASSISTIDO</v>
       </c>
-      <c r="AA51" s="73">
+      <c r="AA51" s="66">
         <v>5.486111111111111E-2</v>
       </c>
       <c r="AB51" s="14"/>
@@ -6295,7 +6296,7 @@
       <c r="F52" s="9" t="s">
         <v>71</v>
       </c>
-      <c r="G52" s="72">
+      <c r="G52" s="65">
         <v>9.930555555555555E-2</v>
       </c>
       <c r="H52" s="6" t="s">
@@ -6333,7 +6334,7 @@
       <c r="Z52" s="6" t="str">
         <v>NÃO ASSISTIDO</v>
       </c>
-      <c r="AA52" s="73">
+      <c r="AA52" s="66">
         <v>5.5555555555555552E-2</v>
       </c>
       <c r="AB52" s="14"/>
@@ -6358,7 +6359,7 @@
       <c r="F53" s="9" t="s">
         <v>81</v>
       </c>
-      <c r="G53" s="72">
+      <c r="G53" s="65">
         <v>0.10486111111111111</v>
       </c>
       <c r="H53" s="6" t="s">
@@ -6396,7 +6397,7 @@
       <c r="Z53" s="6" t="str">
         <v>NÃO ASSISTIDO</v>
       </c>
-      <c r="AA53" s="73">
+      <c r="AA53" s="66">
         <v>5.2777777777777778E-2</v>
       </c>
       <c r="AB53" s="14"/>
@@ -6421,7 +6422,7 @@
       <c r="F54" s="9">
         <v>9</v>
       </c>
-      <c r="G54" s="72">
+      <c r="G54" s="65">
         <v>0.11666666666666665</v>
       </c>
       <c r="H54" s="6" t="s">
@@ -6459,7 +6460,7 @@
       <c r="Z54" s="6" t="str">
         <v>ASSISTIDO</v>
       </c>
-      <c r="AA54" s="73">
+      <c r="AA54" s="66">
         <v>5.7638888888888885E-2</v>
       </c>
       <c r="AB54" s="14"/>
@@ -6484,7 +6485,7 @@
       <c r="F55" s="9" t="s">
         <v>71</v>
       </c>
-      <c r="G55" s="72">
+      <c r="G55" s="65">
         <v>9.7916666666666666E-2</v>
       </c>
       <c r="H55" s="6" t="s">
@@ -6522,7 +6523,7 @@
       <c r="Z55" s="6" t="str">
         <v>NÃO ASSISTIDO</v>
       </c>
-      <c r="AA55" s="73">
+      <c r="AA55" s="66">
         <v>6.1111111111111116E-2</v>
       </c>
       <c r="AB55" s="14"/>
@@ -6547,7 +6548,7 @@
       <c r="F56" s="9">
         <v>8</v>
       </c>
-      <c r="G56" s="72">
+      <c r="G56" s="65">
         <v>8.9583333333333334E-2</v>
       </c>
       <c r="H56" s="6" t="s">
@@ -6585,7 +6586,7 @@
       <c r="Z56" s="6" t="str">
         <v>ASSISTIDO</v>
       </c>
-      <c r="AA56" s="73">
+      <c r="AA56" s="66">
         <v>6.5972222222222224E-2</v>
       </c>
       <c r="AB56" s="14"/>
@@ -6610,7 +6611,7 @@
       <c r="F57" s="9" t="s">
         <v>71</v>
       </c>
-      <c r="G57" s="72">
+      <c r="G57" s="65">
         <v>6.3194444444444442E-2</v>
       </c>
       <c r="H57" s="6" t="s">
@@ -6648,7 +6649,7 @@
       <c r="Z57" s="6" t="str">
         <v>NÃO ASSISTIDO</v>
       </c>
-      <c r="AA57" s="72">
+      <c r="AA57" s="65">
         <v>6.9444444444444434E-2</v>
       </c>
       <c r="AB57" s="14"/>
@@ -6673,7 +6674,7 @@
       <c r="F58" s="9">
         <v>8</v>
       </c>
-      <c r="G58" s="72">
+      <c r="G58" s="65">
         <v>6.25E-2</v>
       </c>
       <c r="H58" s="6" t="s">
@@ -6710,7 +6711,7 @@
       <c r="Z58" s="43" t="str">
         <v>NÃO ASSISTIDO</v>
       </c>
-      <c r="AA58" s="74">
+      <c r="AA58" s="67">
         <v>6.9444444444444434E-2</v>
       </c>
     </row>
@@ -6734,7 +6735,7 @@
       <c r="F59" s="9">
         <v>10</v>
       </c>
-      <c r="G59" s="72">
+      <c r="G59" s="65">
         <v>5.4166666666666669E-2</v>
       </c>
       <c r="H59" s="6" t="s">
@@ -6771,7 +6772,7 @@
       <c r="Z59" s="6" t="str">
         <v>NÃO ASSISTIDO</v>
       </c>
-      <c r="AA59" s="72">
+      <c r="AA59" s="65">
         <v>6.9444444444444434E-2</v>
       </c>
     </row>
@@ -6795,7 +6796,7 @@
       <c r="F60" s="9">
         <v>9</v>
       </c>
-      <c r="G60" s="72">
+      <c r="G60" s="65">
         <v>5.2083333333333336E-2</v>
       </c>
       <c r="H60" s="6" t="s">
@@ -6832,7 +6833,7 @@
       <c r="Z60" s="6" t="str">
         <v>NÃO ASSISTIDO</v>
       </c>
-      <c r="AA60" s="72">
+      <c r="AA60" s="65">
         <v>6.9444444444444434E-2</v>
       </c>
     </row>
@@ -6856,7 +6857,7 @@
       <c r="F61" s="9">
         <v>9</v>
       </c>
-      <c r="G61" s="72">
+      <c r="G61" s="65">
         <v>5.5555555555555552E-2</v>
       </c>
       <c r="H61" s="6" t="s">
@@ -6893,7 +6894,7 @@
       <c r="Z61" s="6" t="str">
         <v>NÃO ASSISTIDO</v>
       </c>
-      <c r="AA61" s="72">
+      <c r="AA61" s="65">
         <v>6.9444444444444434E-2</v>
       </c>
     </row>
@@ -6917,7 +6918,7 @@
       <c r="F62" s="9">
         <v>9</v>
       </c>
-      <c r="G62" s="72">
+      <c r="G62" s="65">
         <v>5.2083333333333336E-2</v>
       </c>
       <c r="H62" s="6" t="s">
@@ -6954,7 +6955,7 @@
       <c r="Z62" s="6" t="str">
         <v>NÃO ASSISTIDO</v>
       </c>
-      <c r="AA62" s="72">
+      <c r="AA62" s="65">
         <v>6.9444444444444434E-2</v>
       </c>
     </row>
@@ -6978,7 +6979,7 @@
       <c r="F63" s="9">
         <v>6</v>
       </c>
-      <c r="G63" s="72">
+      <c r="G63" s="65">
         <v>4.9999999999999996E-2</v>
       </c>
       <c r="H63" s="6" t="s">
@@ -7015,7 +7016,7 @@
       <c r="Z63" s="6" t="str">
         <v>NÃO ASSISTIDO</v>
       </c>
-      <c r="AA63" s="72">
+      <c r="AA63" s="65">
         <v>6.9444444444444434E-2</v>
       </c>
     </row>
@@ -7039,7 +7040,7 @@
       <c r="F64" s="9">
         <v>5</v>
       </c>
-      <c r="G64" s="72">
+      <c r="G64" s="65">
         <v>5.2083333333333336E-2</v>
       </c>
       <c r="H64" s="6" t="s">
@@ -7076,7 +7077,7 @@
       <c r="Z64" s="6" t="str">
         <v>NÃO ASSISTIDO</v>
       </c>
-      <c r="AA64" s="72">
+      <c r="AA64" s="65">
         <v>6.9444444444444434E-2</v>
       </c>
     </row>
@@ -7100,7 +7101,7 @@
       <c r="F65" s="9">
         <v>6</v>
       </c>
-      <c r="G65" s="72">
+      <c r="G65" s="65">
         <v>5.1388888888888894E-2</v>
       </c>
       <c r="H65" s="6" t="s">
@@ -7137,7 +7138,7 @@
       <c r="Z65" s="6" t="str">
         <v>NÃO ASSISTIDO</v>
       </c>
-      <c r="AA65" s="72">
+      <c r="AA65" s="65">
         <v>6.9444444444444434E-2</v>
       </c>
     </row>
@@ -7161,7 +7162,7 @@
       <c r="F66" s="9">
         <v>6</v>
       </c>
-      <c r="G66" s="72">
+      <c r="G66" s="65">
         <v>5.2083333333333336E-2</v>
       </c>
       <c r="H66" s="6" t="s">
@@ -7198,7 +7199,7 @@
       <c r="Z66" s="6" t="str">
         <v>NÃO ASSISTIDO</v>
       </c>
-      <c r="AA66" s="72">
+      <c r="AA66" s="65">
         <v>6.9444444444444434E-2</v>
       </c>
     </row>
@@ -7222,7 +7223,7 @@
       <c r="F67" s="9" t="s">
         <v>71</v>
       </c>
-      <c r="G67" s="72">
+      <c r="G67" s="65">
         <v>5.486111111111111E-2</v>
       </c>
       <c r="H67" s="6" t="s">
@@ -7259,7 +7260,7 @@
       <c r="Z67" s="6" t="str">
         <v>NÃO ASSISTIDO</v>
       </c>
-      <c r="AA67" s="72">
+      <c r="AA67" s="65">
         <v>6.9444444444444434E-2</v>
       </c>
     </row>
@@ -7283,7 +7284,7 @@
       <c r="F68" s="9">
         <v>7</v>
       </c>
-      <c r="G68" s="72">
+      <c r="G68" s="65">
         <v>5.5555555555555552E-2</v>
       </c>
       <c r="H68" s="6" t="s">
@@ -7320,7 +7321,7 @@
       <c r="Z68" s="6" t="str">
         <v>NÃO ASSISTIDO</v>
       </c>
-      <c r="AA68" s="72">
+      <c r="AA68" s="65">
         <v>6.9444444444444434E-2</v>
       </c>
     </row>
@@ -7344,7 +7345,7 @@
       <c r="F69" s="9">
         <v>7</v>
       </c>
-      <c r="G69" s="72">
+      <c r="G69" s="65">
         <v>6.25E-2</v>
       </c>
       <c r="H69" s="6" t="s">
@@ -7381,7 +7382,7 @@
       <c r="Z69" s="6" t="str">
         <v>ASSISTIDO</v>
       </c>
-      <c r="AA69" s="72">
+      <c r="AA69" s="65">
         <v>6.9444444444444434E-2</v>
       </c>
     </row>
@@ -7405,7 +7406,7 @@
       <c r="F70" s="9">
         <v>8</v>
       </c>
-      <c r="G70" s="72">
+      <c r="G70" s="65">
         <v>5.2083333333333336E-2</v>
       </c>
       <c r="H70" s="6" t="s">
@@ -7442,7 +7443,7 @@
       <c r="Z70" s="6" t="str">
         <v>NÃO ASSISTIDO</v>
       </c>
-      <c r="AA70" s="72">
+      <c r="AA70" s="65">
         <v>6.9444444444444434E-2</v>
       </c>
     </row>
@@ -7466,7 +7467,7 @@
       <c r="F71" s="9" t="s">
         <v>73</v>
       </c>
-      <c r="G71" s="72">
+      <c r="G71" s="65">
         <v>5.2777777777777778E-2</v>
       </c>
       <c r="H71" s="6" t="s">
@@ -7503,7 +7504,7 @@
       <c r="Z71" s="6" t="str">
         <v>NÃO ASSISTIDO</v>
       </c>
-      <c r="AA71" s="72">
+      <c r="AA71" s="65">
         <v>6.9444444444444434E-2</v>
       </c>
     </row>
@@ -7527,7 +7528,7 @@
       <c r="F72" s="9" t="s">
         <v>81</v>
       </c>
-      <c r="G72" s="72">
+      <c r="G72" s="65">
         <v>5.347222222222222E-2</v>
       </c>
       <c r="H72" s="6" t="s">
@@ -7564,7 +7565,7 @@
       <c r="Z72" s="6" t="str">
         <v>NÃO ASSISTIDO</v>
       </c>
-      <c r="AA72" s="72">
+      <c r="AA72" s="65">
         <v>6.9444444444444434E-2</v>
       </c>
     </row>
@@ -7588,7 +7589,7 @@
       <c r="F73" s="9">
         <v>9</v>
       </c>
-      <c r="G73" s="72">
+      <c r="G73" s="65">
         <v>5.347222222222222E-2</v>
       </c>
       <c r="H73" s="6" t="s">
@@ -7625,7 +7626,7 @@
       <c r="Z73" s="6" t="str">
         <v>NÃO ASSISTIDO</v>
       </c>
-      <c r="AA73" s="72">
+      <c r="AA73" s="65">
         <v>6.9444444444444434E-2</v>
       </c>
     </row>
@@ -7649,7 +7650,7 @@
       <c r="F74" s="9">
         <v>8</v>
       </c>
-      <c r="G74" s="72">
+      <c r="G74" s="65">
         <v>5.2777777777777778E-2</v>
       </c>
       <c r="H74" s="6" t="s">
@@ -7686,7 +7687,7 @@
       <c r="Z74" s="6" t="str">
         <v>NÃO ASSISTIDO</v>
       </c>
-      <c r="AA74" s="72">
+      <c r="AA74" s="65">
         <v>6.9444444444444434E-2</v>
       </c>
     </row>
@@ -7710,7 +7711,7 @@
       <c r="F75" s="9">
         <v>6</v>
       </c>
-      <c r="G75" s="72">
+      <c r="G75" s="65">
         <v>5.486111111111111E-2</v>
       </c>
       <c r="H75" s="6" t="s">
@@ -7747,7 +7748,7 @@
       <c r="Z75" s="6" t="str">
         <v>NÃO ASSISTIDO</v>
       </c>
-      <c r="AA75" s="72">
+      <c r="AA75" s="65">
         <v>6.9444444444444434E-2</v>
       </c>
     </row>
@@ -7771,7 +7772,7 @@
       <c r="F76" s="9">
         <v>6</v>
       </c>
-      <c r="G76" s="72">
+      <c r="G76" s="65">
         <v>5.8333333333333327E-2</v>
       </c>
       <c r="H76" s="6" t="s">
@@ -7799,14 +7800,14 @@
         <f t="shared" si="11"/>
         <v>75</v>
       </c>
-      <c r="X76" s="63" t="s">
+      <c r="X76" s="71" t="s">
         <v>206</v>
       </c>
-      <c r="Y76" s="64"/>
-      <c r="Z76" s="65"/>
-      <c r="AA76" s="75">
+      <c r="Y76" s="72"/>
+      <c r="Z76" s="73"/>
+      <c r="AA76" s="77">
         <f>SUMIF($Z$6:$Z$75,"ASSISTIDO",$AA$6:$AA$75)</f>
-        <v>3.0472222222222221</v>
+        <v>3.098611111111111</v>
       </c>
     </row>
     <row r="77" spans="1:27" x14ac:dyDescent="0.25">
@@ -7829,7 +7830,7 @@
       <c r="F77" s="9" t="s">
         <v>73</v>
       </c>
-      <c r="G77" s="72">
+      <c r="G77" s="65">
         <v>5.4166666666666669E-2</v>
       </c>
       <c r="H77" s="6" t="s">
@@ -7878,7 +7879,7 @@
       <c r="F78" s="9">
         <v>7</v>
       </c>
-      <c r="G78" s="72">
+      <c r="G78" s="65">
         <v>45</v>
       </c>
       <c r="H78" s="6" t="s">
@@ -7927,7 +7928,7 @@
       <c r="F79" s="9">
         <v>9</v>
       </c>
-      <c r="G79" s="72">
+      <c r="G79" s="65">
         <v>5.4166666666666669E-2</v>
       </c>
       <c r="H79" s="6" t="s">
@@ -7976,7 +7977,7 @@
       <c r="F80" s="9">
         <v>7</v>
       </c>
-      <c r="G80" s="72">
+      <c r="G80" s="65">
         <v>5.8333333333333327E-2</v>
       </c>
       <c r="H80" s="6" t="s">
@@ -8025,7 +8026,7 @@
       <c r="F81" s="9">
         <v>4</v>
       </c>
-      <c r="G81" s="72">
+      <c r="G81" s="65">
         <v>5.1388888888888894E-2</v>
       </c>
       <c r="H81" s="6" t="s">
@@ -8074,7 +8075,7 @@
       <c r="F82" s="9">
         <v>3</v>
       </c>
-      <c r="G82" s="72">
+      <c r="G82" s="65">
         <v>5.5555555555555552E-2</v>
       </c>
       <c r="H82" s="6" t="s">
@@ -8123,7 +8124,7 @@
       <c r="F83" s="9">
         <v>6</v>
       </c>
-      <c r="G83" s="72">
+      <c r="G83" s="65">
         <v>5.486111111111111E-2</v>
       </c>
       <c r="H83" s="6" t="s">
@@ -8172,7 +8173,7 @@
       <c r="F84" s="9">
         <v>7</v>
       </c>
-      <c r="G84" s="72">
+      <c r="G84" s="65">
         <v>5.2083333333333336E-2</v>
       </c>
       <c r="H84" s="6" t="s">
@@ -8221,7 +8222,7 @@
       <c r="F85" s="9">
         <v>4</v>
       </c>
-      <c r="G85" s="72">
+      <c r="G85" s="65">
         <v>5.6944444444444443E-2</v>
       </c>
       <c r="H85" s="6" t="s">
@@ -8270,7 +8271,7 @@
       <c r="F86" s="9">
         <v>7</v>
       </c>
-      <c r="G86" s="72">
+      <c r="G86" s="65">
         <v>5.486111111111111E-2</v>
       </c>
       <c r="H86" s="6" t="s">
@@ -8319,7 +8320,7 @@
       <c r="F87" s="9">
         <v>4</v>
       </c>
-      <c r="G87" s="72">
+      <c r="G87" s="65">
         <v>5.4166666666666669E-2</v>
       </c>
       <c r="H87" s="6" t="s">
@@ -8368,7 +8369,7 @@
       <c r="F88" s="9">
         <v>5</v>
       </c>
-      <c r="G88" s="72">
+      <c r="G88" s="65">
         <v>5.2083333333333336E-2</v>
       </c>
       <c r="H88" s="6" t="s">
@@ -8417,7 +8418,7 @@
       <c r="F89" s="9">
         <v>6</v>
       </c>
-      <c r="G89" s="72">
+      <c r="G89" s="65">
         <v>5.347222222222222E-2</v>
       </c>
       <c r="H89" s="6" t="s">
@@ -8466,7 +8467,7 @@
       <c r="F90" s="9">
         <v>4</v>
       </c>
-      <c r="G90" s="72">
+      <c r="G90" s="65">
         <v>4.9999999999999996E-2</v>
       </c>
       <c r="H90" s="6" t="s">
@@ -8515,7 +8516,7 @@
       <c r="F91" s="9">
         <v>0</v>
       </c>
-      <c r="G91" s="72">
+      <c r="G91" s="65">
         <v>5.5555555555555552E-2</v>
       </c>
       <c r="H91" s="6" t="s">
@@ -8564,7 +8565,7 @@
       <c r="F92" s="9">
         <v>8</v>
       </c>
-      <c r="G92" s="72">
+      <c r="G92" s="65">
         <v>5.5555555555555552E-2</v>
       </c>
       <c r="H92" s="6" t="s">
@@ -8613,7 +8614,7 @@
       <c r="F93" s="9">
         <v>6</v>
       </c>
-      <c r="G93" s="72">
+      <c r="G93" s="65">
         <v>5.2777777777777778E-2</v>
       </c>
       <c r="H93" s="6" t="s">
@@ -8662,7 +8663,7 @@
       <c r="F94" s="9">
         <v>10</v>
       </c>
-      <c r="G94" s="72">
+      <c r="G94" s="65">
         <v>5.9722222222222225E-2</v>
       </c>
       <c r="H94" s="6" t="s">
@@ -8711,7 +8712,7 @@
       <c r="F95" s="9">
         <v>8</v>
       </c>
-      <c r="G95" s="72">
+      <c r="G95" s="65">
         <v>6.458333333333334E-2</v>
       </c>
       <c r="H95" s="6" t="s">
@@ -8760,7 +8761,7 @@
       <c r="F96" s="9">
         <v>6</v>
       </c>
-      <c r="G96" s="72">
+      <c r="G96" s="65">
         <v>6.458333333333334E-2</v>
       </c>
       <c r="H96" s="6" t="s">
@@ -8809,7 +8810,7 @@
       <c r="F97" s="9">
         <v>9</v>
       </c>
-      <c r="G97" s="72">
+      <c r="G97" s="65">
         <v>5.6250000000000001E-2</v>
       </c>
       <c r="H97" s="6" t="s">
@@ -8858,7 +8859,7 @@
       <c r="F98" s="9" t="s">
         <v>71</v>
       </c>
-      <c r="G98" s="72">
+      <c r="G98" s="65">
         <v>5.1388888888888894E-2</v>
       </c>
       <c r="H98" s="6" t="s">
@@ -8907,7 +8908,7 @@
       <c r="F99" s="9" t="s">
         <v>81</v>
       </c>
-      <c r="G99" s="72">
+      <c r="G99" s="65">
         <v>6.5972222222222224E-2</v>
       </c>
       <c r="H99" s="6" t="s">
@@ -8956,7 +8957,7 @@
       <c r="F100" s="9" t="s">
         <v>81</v>
       </c>
-      <c r="G100" s="72">
+      <c r="G100" s="65">
         <v>6.9444444444444434E-2</v>
       </c>
       <c r="H100" s="6" t="s">
@@ -9005,7 +9006,7 @@
       <c r="F101" s="9">
         <v>7</v>
       </c>
-      <c r="G101" s="72">
+      <c r="G101" s="65">
         <v>5.4166666666666669E-2</v>
       </c>
       <c r="H101" s="6" t="s">
@@ -9054,7 +9055,7 @@
       <c r="F102" s="9">
         <v>7</v>
       </c>
-      <c r="G102" s="72">
+      <c r="G102" s="65">
         <v>5.9722222222222225E-2</v>
       </c>
       <c r="H102" s="6" t="s">
@@ -9103,7 +9104,7 @@
       <c r="F103" s="9" t="s">
         <v>71</v>
       </c>
-      <c r="G103" s="72">
+      <c r="G103" s="65">
         <v>6.3194444444444442E-2</v>
       </c>
       <c r="H103" s="6" t="s">
@@ -9152,7 +9153,7 @@
       <c r="F104" s="9">
         <v>8</v>
       </c>
-      <c r="G104" s="72">
+      <c r="G104" s="65">
         <v>6.1805555555555558E-2</v>
       </c>
       <c r="H104" s="6" t="s">
@@ -9201,7 +9202,7 @@
       <c r="F105" s="9">
         <v>8</v>
       </c>
-      <c r="G105" s="72">
+      <c r="G105" s="65">
         <v>6.7361111111111108E-2</v>
       </c>
       <c r="H105" s="6" t="s">
@@ -9244,7 +9245,13 @@
       <c r="D106" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="G106" s="72">
+      <c r="E106" s="7">
+        <v>45137</v>
+      </c>
+      <c r="F106" s="9">
+        <v>8</v>
+      </c>
+      <c r="G106" s="65">
         <v>5.1388888888888894E-2</v>
       </c>
       <c r="H106" s="6" t="s">
@@ -9262,11 +9269,11 @@
       </c>
       <c r="L106" s="23">
         <f t="shared" si="12"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M106" s="25" t="str">
         <f t="shared" si="13"/>
-        <v>NÃO ASSISTIDO</v>
+        <v>ASSISTIDO</v>
       </c>
       <c r="N106" s="6">
         <f t="shared" si="11"/>
@@ -9293,7 +9300,7 @@
       <c r="F107" s="9" t="s">
         <v>71</v>
       </c>
-      <c r="G107" s="72">
+      <c r="G107" s="65">
         <v>6.5972222222222224E-2</v>
       </c>
       <c r="H107" s="6" t="s">
@@ -9336,7 +9343,7 @@
       <c r="D108" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="G108" s="72">
+      <c r="G108" s="65">
         <v>6.7361111111111108E-2</v>
       </c>
       <c r="H108" s="6" t="s">
@@ -9385,7 +9392,7 @@
       <c r="F109" s="9">
         <v>9</v>
       </c>
-      <c r="G109" s="72">
+      <c r="G109" s="65">
         <v>7.1527777777777787E-2</v>
       </c>
       <c r="H109" s="6" t="s">
@@ -9434,7 +9441,7 @@
       <c r="F110" s="9" t="s">
         <v>71</v>
       </c>
-      <c r="G110" s="72">
+      <c r="G110" s="65">
         <v>6.6666666666666666E-2</v>
       </c>
       <c r="H110" s="6" t="s">
@@ -9483,7 +9490,7 @@
       <c r="F111" s="9">
         <v>9</v>
       </c>
-      <c r="G111" s="72">
+      <c r="G111" s="65">
         <v>7.2222222222222229E-2</v>
       </c>
       <c r="H111" s="6" t="s">
@@ -9532,7 +9539,7 @@
       <c r="F112" s="9">
         <v>9</v>
       </c>
-      <c r="G112" s="72">
+      <c r="G112" s="65">
         <v>6.805555555555555E-2</v>
       </c>
       <c r="H112" s="6" t="s">
@@ -9581,7 +9588,7 @@
       <c r="F113" s="9" t="s">
         <v>71</v>
       </c>
-      <c r="G113" s="72">
+      <c r="G113" s="65">
         <v>7.7083333333333337E-2</v>
       </c>
       <c r="H113" s="6" t="s">
@@ -9630,7 +9637,7 @@
       <c r="F114" s="9">
         <v>9</v>
       </c>
-      <c r="G114" s="72">
+      <c r="G114" s="65">
         <v>6.9444444444444434E-2</v>
       </c>
       <c r="H114" s="6" t="s">
@@ -9679,7 +9686,7 @@
       <c r="F115" s="9">
         <v>9</v>
       </c>
-      <c r="G115" s="72">
+      <c r="G115" s="65">
         <v>6.9444444444444434E-2</v>
       </c>
       <c r="H115" s="6" t="s">
@@ -9728,7 +9735,7 @@
       <c r="F116" s="9">
         <v>8</v>
       </c>
-      <c r="G116" s="72">
+      <c r="G116" s="65">
         <v>6.7361111111111108E-2</v>
       </c>
       <c r="H116" s="6" t="s">
@@ -9771,7 +9778,7 @@
       <c r="D117" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="G117" s="72">
+      <c r="G117" s="65">
         <v>6.6666666666666666E-2</v>
       </c>
       <c r="H117" s="6" t="s">
@@ -9820,7 +9827,7 @@
       <c r="F118" s="9" t="s">
         <v>71</v>
       </c>
-      <c r="G118" s="72">
+      <c r="G118" s="65">
         <v>5.2777777777777778E-2</v>
       </c>
       <c r="H118" s="6" t="s">
@@ -9869,7 +9876,7 @@
       <c r="F119" s="9" t="s">
         <v>71</v>
       </c>
-      <c r="G119" s="72">
+      <c r="G119" s="65">
         <v>7.0833333333333331E-2</v>
       </c>
       <c r="H119" s="6" t="s">
@@ -9918,7 +9925,7 @@
       <c r="F120" s="9" t="s">
         <v>71</v>
       </c>
-      <c r="G120" s="72">
+      <c r="G120" s="65">
         <v>5.2777777777777778E-2</v>
       </c>
       <c r="H120" s="6" t="s">
@@ -9964,7 +9971,7 @@
       <c r="F121" s="9">
         <v>9</v>
       </c>
-      <c r="G121" s="72">
+      <c r="G121" s="65">
         <v>5.4166666666666669E-2</v>
       </c>
       <c r="H121" s="6" t="s">
@@ -10013,7 +10020,7 @@
       <c r="F122" s="9" t="s">
         <v>71</v>
       </c>
-      <c r="G122" s="72">
+      <c r="G122" s="65">
         <v>5.4166666666666669E-2</v>
       </c>
       <c r="H122" s="6" t="s">
@@ -10056,7 +10063,7 @@
       <c r="D123" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="G123" s="72">
+      <c r="G123" s="65">
         <v>5.9722222222222225E-2</v>
       </c>
       <c r="H123" s="6" t="s">
@@ -10105,7 +10112,7 @@
       <c r="F124" s="9">
         <v>10</v>
       </c>
-      <c r="G124" s="72">
+      <c r="G124" s="65">
         <v>5.6250000000000001E-2</v>
       </c>
       <c r="H124" s="6" t="s">
@@ -10148,7 +10155,7 @@
       <c r="D125" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="G125" s="72">
+      <c r="G125" s="65">
         <v>6.5972222222222224E-2</v>
       </c>
       <c r="H125" s="6" t="s">
@@ -10197,7 +10204,7 @@
       <c r="F126" s="9">
         <v>8</v>
       </c>
-      <c r="G126" s="72">
+      <c r="G126" s="65">
         <v>4.4444444444444446E-2</v>
       </c>
       <c r="H126" s="6" t="s">
@@ -10240,7 +10247,7 @@
       <c r="D127" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="G127" s="72">
+      <c r="G127" s="65">
         <v>5.486111111111111E-2</v>
       </c>
       <c r="H127" s="6" t="s">
@@ -10283,7 +10290,7 @@
       <c r="D128" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="G128" s="72">
+      <c r="G128" s="65">
         <v>5.5555555555555552E-2</v>
       </c>
       <c r="H128" s="6" t="s">
@@ -10326,7 +10333,7 @@
       <c r="D129" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="G129" s="72">
+      <c r="G129" s="65">
         <v>5.2777777777777778E-2</v>
       </c>
       <c r="H129" s="6" t="s">
@@ -10375,7 +10382,7 @@
       <c r="F130" s="9">
         <v>9</v>
       </c>
-      <c r="G130" s="72">
+      <c r="G130" s="65">
         <v>6.458333333333334E-2</v>
       </c>
       <c r="H130" s="6" t="s">
@@ -10424,7 +10431,7 @@
       <c r="F131" s="9">
         <v>9</v>
       </c>
-      <c r="G131" s="72">
+      <c r="G131" s="65">
         <v>8.1250000000000003E-2</v>
       </c>
       <c r="H131" s="6" t="s">
@@ -10473,7 +10480,7 @@
       <c r="F132" s="9">
         <v>8</v>
       </c>
-      <c r="G132" s="72">
+      <c r="G132" s="65">
         <v>7.3611111111111113E-2</v>
       </c>
       <c r="H132" s="6" t="s">
@@ -10522,7 +10529,7 @@
       <c r="F133" s="9" t="s">
         <v>72</v>
       </c>
-      <c r="G133" s="72">
+      <c r="G133" s="65">
         <v>7.5694444444444439E-2</v>
       </c>
       <c r="H133" s="6" t="s">
@@ -10565,7 +10572,7 @@
       <c r="D134" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="G134" s="72">
+      <c r="G134" s="65">
         <v>6.458333333333334E-2</v>
       </c>
       <c r="H134" s="6" t="s">
@@ -10614,7 +10621,7 @@
       <c r="F135" s="9" t="s">
         <v>71</v>
       </c>
-      <c r="G135" s="72">
+      <c r="G135" s="65">
         <v>6.6666666666666666E-2</v>
       </c>
       <c r="H135" s="6" t="s">
@@ -10663,7 +10670,7 @@
       <c r="F136" s="9" t="s">
         <v>168</v>
       </c>
-      <c r="G136" s="72">
+      <c r="G136" s="65">
         <v>7.0833333333333331E-2</v>
       </c>
       <c r="H136" s="6" t="s">
@@ -10706,7 +10713,7 @@
       <c r="D137" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="G137" s="72">
+      <c r="G137" s="65">
         <v>6.8749999999999992E-2</v>
       </c>
       <c r="H137" s="6" t="s">
@@ -10752,7 +10759,7 @@
       <c r="F138" s="9">
         <v>9</v>
       </c>
-      <c r="G138" s="72">
+      <c r="G138" s="65">
         <v>5.7638888888888885E-2</v>
       </c>
       <c r="H138" s="6" t="s">
@@ -10795,7 +10802,7 @@
       <c r="D139" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="G139" s="72">
+      <c r="G139" s="65">
         <v>6.1111111111111116E-2</v>
       </c>
       <c r="H139" s="6" t="s">
@@ -10844,7 +10851,7 @@
       <c r="F140" s="9">
         <v>10</v>
       </c>
-      <c r="G140" s="72">
+      <c r="G140" s="65">
         <v>7.9166666666666663E-2</v>
       </c>
       <c r="H140" s="6" t="s">
@@ -10893,7 +10900,7 @@
       <c r="F141" s="9">
         <v>9</v>
       </c>
-      <c r="G141" s="72">
+      <c r="G141" s="65">
         <v>6.5277777777777782E-2</v>
       </c>
       <c r="H141" s="6" t="s">
@@ -10942,7 +10949,7 @@
       <c r="F142" s="9" t="s">
         <v>71</v>
       </c>
-      <c r="G142" s="72">
+      <c r="G142" s="65">
         <v>5.9027777777777783E-2</v>
       </c>
       <c r="H142" s="6" t="s">
@@ -10985,7 +10992,7 @@
       <c r="D143" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="G143" s="72">
+      <c r="G143" s="65">
         <v>5.9722222222222225E-2</v>
       </c>
       <c r="H143" s="6" t="s">
@@ -11034,7 +11041,7 @@
       <c r="F144" s="9">
         <v>9</v>
       </c>
-      <c r="G144" s="72">
+      <c r="G144" s="65">
         <v>7.6388888888888895E-2</v>
       </c>
       <c r="H144" s="6" t="s">
@@ -11083,7 +11090,7 @@
       <c r="F145" s="9" t="s">
         <v>72</v>
       </c>
-      <c r="G145" s="72">
+      <c r="G145" s="65">
         <v>7.6388888888888895E-2</v>
       </c>
       <c r="H145" s="6" t="s">
@@ -11132,7 +11139,7 @@
       <c r="F146" s="9">
         <v>8</v>
       </c>
-      <c r="G146" s="72">
+      <c r="G146" s="65">
         <v>6.5972222222222224E-2</v>
       </c>
       <c r="H146" s="6" t="s">
@@ -11181,7 +11188,7 @@
       <c r="F147" s="9" t="s">
         <v>71</v>
       </c>
-      <c r="G147" s="72">
+      <c r="G147" s="65">
         <v>6.805555555555555E-2</v>
       </c>
       <c r="H147" s="6" t="s">
@@ -11230,7 +11237,7 @@
       <c r="F148" s="9">
         <v>9</v>
       </c>
-      <c r="G148" s="72">
+      <c r="G148" s="65">
         <v>6.5972222222222224E-2</v>
       </c>
       <c r="H148" s="6" t="s">
@@ -11279,7 +11286,7 @@
       <c r="F149" s="9">
         <v>9</v>
       </c>
-      <c r="G149" s="72">
+      <c r="G149" s="65">
         <v>6.3888888888888884E-2</v>
       </c>
       <c r="H149" s="6" t="s">
@@ -11328,7 +11335,7 @@
       <c r="F150" s="9" t="s">
         <v>72</v>
       </c>
-      <c r="G150" s="72">
+      <c r="G150" s="65">
         <v>7.7777777777777779E-2</v>
       </c>
       <c r="H150" s="6" t="s">
@@ -11377,7 +11384,7 @@
       <c r="F151" s="9" t="s">
         <v>72</v>
       </c>
-      <c r="G151" s="72">
+      <c r="G151" s="65">
         <v>8.3333333333333329E-2</v>
       </c>
       <c r="H151" s="6" t="s">
@@ -11426,7 +11433,7 @@
       <c r="F152" s="9" t="s">
         <v>73</v>
       </c>
-      <c r="G152" s="72">
+      <c r="G152" s="65">
         <v>8.4027777777777771E-2</v>
       </c>
       <c r="H152" s="6" t="s">
@@ -11475,7 +11482,7 @@
       <c r="F153" s="9">
         <v>8</v>
       </c>
-      <c r="G153" s="72">
+      <c r="G153" s="65">
         <v>8.819444444444445E-2</v>
       </c>
       <c r="H153" s="6" t="s">
@@ -11524,7 +11531,7 @@
       <c r="F154" s="9" t="s">
         <v>73</v>
       </c>
-      <c r="G154" s="72">
+      <c r="G154" s="65">
         <v>9.6527777777777768E-2</v>
       </c>
       <c r="H154" s="6" t="s">
@@ -11573,7 +11580,7 @@
       <c r="F155" s="9">
         <v>9</v>
       </c>
-      <c r="G155" s="72">
+      <c r="G155" s="65">
         <v>8.3333333333333329E-2</v>
       </c>
       <c r="H155" s="6" t="s">
@@ -11622,7 +11629,7 @@
       <c r="F156" s="9">
         <v>9</v>
       </c>
-      <c r="G156" s="72">
+      <c r="G156" s="65">
         <v>8.3333333333333329E-2</v>
       </c>
       <c r="H156" s="6" t="s">
@@ -11666,7 +11673,7 @@
         <v>6</v>
       </c>
       <c r="E157" s="7"/>
-      <c r="G157" s="72">
+      <c r="G157" s="65">
         <v>7.2916666666666671E-2</v>
       </c>
       <c r="H157" s="6" t="s">
@@ -11709,7 +11716,7 @@
         <v>6</v>
       </c>
       <c r="E158" s="7"/>
-      <c r="G158" s="72">
+      <c r="G158" s="65">
         <v>6.9444444444444434E-2</v>
       </c>
       <c r="H158" s="6" t="s">
@@ -11752,7 +11759,7 @@
         <v>9</v>
       </c>
       <c r="E159" s="7"/>
-      <c r="G159" s="72">
+      <c r="G159" s="65">
         <v>6.9444444444444434E-2</v>
       </c>
       <c r="H159" s="6" t="s">
@@ -11795,7 +11802,7 @@
         <v>9</v>
       </c>
       <c r="E160" s="7"/>
-      <c r="G160" s="72">
+      <c r="G160" s="65">
         <v>6.9444444444444434E-2</v>
       </c>
       <c r="H160" s="6" t="s">
@@ -11838,7 +11845,7 @@
         <v>9</v>
       </c>
       <c r="E161" s="7"/>
-      <c r="G161" s="72">
+      <c r="G161" s="65">
         <v>6.9444444444444434E-2</v>
       </c>
       <c r="H161" s="6" t="s">
@@ -11881,7 +11888,7 @@
         <v>9</v>
       </c>
       <c r="E162" s="7"/>
-      <c r="G162" s="72">
+      <c r="G162" s="65">
         <v>6.9444444444444434E-2</v>
       </c>
       <c r="H162" s="6" t="s">
@@ -11924,7 +11931,7 @@
         <v>9</v>
       </c>
       <c r="E163" s="7"/>
-      <c r="G163" s="72">
+      <c r="G163" s="65">
         <v>6.9444444444444434E-2</v>
       </c>
       <c r="H163" s="6" t="s">
@@ -11967,7 +11974,7 @@
         <v>9</v>
       </c>
       <c r="E164" s="7"/>
-      <c r="G164" s="72">
+      <c r="G164" s="65">
         <v>6.9444444444444434E-2</v>
       </c>
       <c r="H164" s="6" t="s">
@@ -12010,7 +12017,7 @@
         <v>9</v>
       </c>
       <c r="E165" s="7"/>
-      <c r="G165" s="72">
+      <c r="G165" s="65">
         <v>6.9444444444444434E-2</v>
       </c>
       <c r="H165" s="6" t="s">
@@ -12053,7 +12060,7 @@
         <v>9</v>
       </c>
       <c r="E166" s="7"/>
-      <c r="G166" s="72">
+      <c r="G166" s="65">
         <v>6.9444444444444434E-2</v>
       </c>
       <c r="H166" s="6" t="s">
@@ -12096,7 +12103,7 @@
         <v>9</v>
       </c>
       <c r="E167" s="7"/>
-      <c r="G167" s="72">
+      <c r="G167" s="65">
         <v>6.9444444444444434E-2</v>
       </c>
       <c r="H167" s="6" t="s">
@@ -12139,7 +12146,7 @@
         <v>9</v>
       </c>
       <c r="E168" s="7"/>
-      <c r="G168" s="72">
+      <c r="G168" s="65">
         <v>6.9444444444444434E-2</v>
       </c>
       <c r="H168" s="6" t="s">
@@ -12182,7 +12189,7 @@
         <v>9</v>
       </c>
       <c r="E169" s="7"/>
-      <c r="G169" s="72">
+      <c r="G169" s="65">
         <v>6.9444444444444434E-2</v>
       </c>
       <c r="H169" s="6" t="s">
@@ -12225,7 +12232,7 @@
         <v>9</v>
       </c>
       <c r="E170" s="7"/>
-      <c r="G170" s="72">
+      <c r="G170" s="65">
         <v>6.9444444444444434E-2</v>
       </c>
       <c r="H170" s="6" t="s">
@@ -12273,7 +12280,7 @@
       <c r="F171" s="9" t="s">
         <v>71</v>
       </c>
-      <c r="G171" s="72">
+      <c r="G171" s="65">
         <v>6.9444444444444434E-2</v>
       </c>
       <c r="H171" s="6" t="s">
@@ -12316,7 +12323,7 @@
         <v>9</v>
       </c>
       <c r="E172" s="7"/>
-      <c r="G172" s="72">
+      <c r="G172" s="65">
         <v>6.9444444444444434E-2</v>
       </c>
       <c r="H172" s="6" t="s">
@@ -12359,7 +12366,7 @@
         <v>6</v>
       </c>
       <c r="E173" s="7"/>
-      <c r="G173" s="72">
+      <c r="G173" s="65">
         <v>6.9444444444444434E-2</v>
       </c>
       <c r="H173" s="6" t="s">
@@ -12402,7 +12409,7 @@
         <v>6</v>
       </c>
       <c r="E174" s="7"/>
-      <c r="G174" s="72">
+      <c r="G174" s="65">
         <v>6.9444444444444434E-2</v>
       </c>
       <c r="H174" s="6" t="s">
@@ -12445,7 +12452,7 @@
         <v>6</v>
       </c>
       <c r="E175" s="7"/>
-      <c r="G175" s="72">
+      <c r="G175" s="65">
         <v>6.9444444444444434E-2</v>
       </c>
       <c r="H175" s="6" t="s">
@@ -12488,7 +12495,7 @@
         <v>9</v>
       </c>
       <c r="E176" s="7"/>
-      <c r="G176" s="72">
+      <c r="G176" s="65">
         <v>6.9444444444444434E-2</v>
       </c>
       <c r="H176" s="6" t="s">
@@ -12531,7 +12538,7 @@
         <v>6</v>
       </c>
       <c r="E177" s="7"/>
-      <c r="G177" s="72">
+      <c r="G177" s="65">
         <v>6.9444444444444434E-2</v>
       </c>
       <c r="H177" s="6" t="s">
@@ -12574,7 +12581,7 @@
         <v>6</v>
       </c>
       <c r="E178" s="7"/>
-      <c r="G178" s="72">
+      <c r="G178" s="65">
         <v>5.7638888888888885E-2</v>
       </c>
       <c r="H178" s="6" t="s">
@@ -12617,7 +12624,7 @@
         <v>6</v>
       </c>
       <c r="E179" s="7"/>
-      <c r="G179" s="72">
+      <c r="G179" s="65">
         <v>6.25E-2</v>
       </c>
       <c r="H179" s="6" t="s">
@@ -12665,7 +12672,7 @@
       <c r="F180" s="9">
         <v>9</v>
       </c>
-      <c r="G180" s="72">
+      <c r="G180" s="65">
         <v>5.9027777777777783E-2</v>
       </c>
       <c r="H180" s="6" t="s">
@@ -12708,7 +12715,7 @@
         <v>6</v>
       </c>
       <c r="E181" s="7"/>
-      <c r="G181" s="72">
+      <c r="G181" s="65">
         <v>6.0416666666666667E-2</v>
       </c>
       <c r="H181" s="6" t="s">
@@ -12751,7 +12758,7 @@
         <v>6</v>
       </c>
       <c r="E182" s="7"/>
-      <c r="G182" s="72">
+      <c r="G182" s="65">
         <v>5.9722222222222225E-2</v>
       </c>
       <c r="H182" s="6" t="s">
@@ -12794,7 +12801,7 @@
         <v>6</v>
       </c>
       <c r="E183" s="7"/>
-      <c r="G183" s="72">
+      <c r="G183" s="65">
         <v>6.3194444444444442E-2</v>
       </c>
       <c r="H183" s="6" t="s">
@@ -12842,7 +12849,7 @@
       <c r="F184" s="9">
         <v>9</v>
       </c>
-      <c r="G184" s="72">
+      <c r="G184" s="65">
         <v>6.1805555555555558E-2</v>
       </c>
       <c r="H184" s="6" t="s">
@@ -12885,7 +12892,7 @@
         <v>6</v>
       </c>
       <c r="E185" s="7"/>
-      <c r="G185" s="72">
+      <c r="G185" s="65">
         <v>7.0833333333333331E-2</v>
       </c>
       <c r="H185" s="6" t="s">
@@ -12928,7 +12935,7 @@
         <v>6</v>
       </c>
       <c r="E186" s="7"/>
-      <c r="G186" s="72">
+      <c r="G186" s="65">
         <v>6.458333333333334E-2</v>
       </c>
       <c r="H186" s="6" t="s">
@@ -12971,7 +12978,7 @@
         <v>6</v>
       </c>
       <c r="E187" s="7"/>
-      <c r="G187" s="72">
+      <c r="G187" s="65">
         <v>6.6666666666666666E-2</v>
       </c>
       <c r="H187" s="6" t="s">
@@ -13013,8 +13020,13 @@
       <c r="D188" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="E188" s="7"/>
-      <c r="G188" s="72">
+      <c r="E188" s="7">
+        <v>45137</v>
+      </c>
+      <c r="F188" s="9" t="s">
+        <v>72</v>
+      </c>
+      <c r="G188" s="65">
         <v>6.5972222222222224E-2</v>
       </c>
       <c r="H188" s="6" t="s">
@@ -13035,7 +13047,7 @@
       </c>
       <c r="M188" s="25" t="str">
         <f t="shared" si="31"/>
-        <v>NÃO ASSISTIDO</v>
+        <v>ASSISTIDO</v>
       </c>
       <c r="N188" s="6">
         <f t="shared" si="23"/>
@@ -13057,7 +13069,7 @@
         <v>6</v>
       </c>
       <c r="E189" s="7"/>
-      <c r="G189" s="72">
+      <c r="G189" s="65">
         <v>6.6666666666666666E-2</v>
       </c>
       <c r="H189" s="6" t="s">
@@ -13100,7 +13112,7 @@
         <v>6</v>
       </c>
       <c r="E190" s="7"/>
-      <c r="G190" s="72">
+      <c r="G190" s="65">
         <v>6.3888888888888884E-2</v>
       </c>
       <c r="H190" s="6" t="s">
@@ -13143,7 +13155,7 @@
         <v>6</v>
       </c>
       <c r="E191" s="7"/>
-      <c r="G191" s="72">
+      <c r="G191" s="65">
         <v>6.3888888888888884E-2</v>
       </c>
       <c r="H191" s="6" t="s">
@@ -13186,7 +13198,7 @@
         <v>6</v>
       </c>
       <c r="E192" s="7"/>
-      <c r="G192" s="72">
+      <c r="G192" s="65">
         <v>6.5277777777777782E-2</v>
       </c>
       <c r="H192" s="6" t="s">
@@ -13229,7 +13241,7 @@
         <v>6</v>
       </c>
       <c r="E193" s="7"/>
-      <c r="G193" s="72">
+      <c r="G193" s="65">
         <v>6.458333333333334E-2</v>
       </c>
       <c r="H193" s="6" t="s">
@@ -13272,7 +13284,7 @@
         <v>6</v>
       </c>
       <c r="E194" s="7"/>
-      <c r="G194" s="72">
+      <c r="G194" s="65">
         <v>6.7361111111111108E-2</v>
       </c>
       <c r="H194" s="6" t="s">
@@ -13315,7 +13327,7 @@
         <v>6</v>
       </c>
       <c r="E195" s="7"/>
-      <c r="G195" s="72">
+      <c r="G195" s="65">
         <v>6.1805555555555558E-2</v>
       </c>
       <c r="H195" s="6" t="s">
@@ -13358,7 +13370,7 @@
         <v>6</v>
       </c>
       <c r="E196" s="7"/>
-      <c r="G196" s="72">
+      <c r="G196" s="65">
         <v>6.3888888888888884E-2</v>
       </c>
       <c r="H196" s="6" t="s">
@@ -13401,7 +13413,7 @@
         <v>6</v>
       </c>
       <c r="E197" s="7"/>
-      <c r="G197" s="72">
+      <c r="G197" s="65">
         <v>6.3194444444444442E-2</v>
       </c>
       <c r="H197" s="6" t="s">
@@ -13444,7 +13456,7 @@
         <v>6</v>
       </c>
       <c r="E198" s="7"/>
-      <c r="G198" s="72">
+      <c r="G198" s="65">
         <v>6.805555555555555E-2</v>
       </c>
       <c r="H198" s="6" t="s">
@@ -13487,7 +13499,7 @@
         <v>6</v>
       </c>
       <c r="E199" s="7"/>
-      <c r="G199" s="72">
+      <c r="G199" s="65">
         <v>6.5972222222222224E-2</v>
       </c>
       <c r="H199" s="6" t="s">
@@ -13530,7 +13542,7 @@
         <v>6</v>
       </c>
       <c r="E200" s="7"/>
-      <c r="G200" s="72">
+      <c r="G200" s="65">
         <v>6.1111111111111116E-2</v>
       </c>
       <c r="H200" s="6" t="s">
@@ -13573,7 +13585,7 @@
         <v>6</v>
       </c>
       <c r="E201" s="7"/>
-      <c r="G201" s="72">
+      <c r="G201" s="65">
         <v>7.4305555555555555E-2</v>
       </c>
       <c r="H201" s="6" t="s">

</xml_diff>

<commit_message>
Adicionados novos filmes À planilha filmes
</commit_message>
<xml_diff>
--- a/Filmes.xlsx
+++ b/Filmes.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26529"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25601"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Paulo\Documents\Planilhas\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Usuario\Documents\Planilhas\Planilhas\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{92C2C1FC-6F10-48F3-BF7A-D14EE1D04B98}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E4432C70-579C-459F-8516-E4AA7CE16E60}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{AC88744C-D9DF-4ECD-8B9A-C97C8CD0E4BD}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{AC88744C-D9DF-4ECD-8B9A-C97C8CD0E4BD}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
@@ -39,9 +39,10 @@
 </file>
 
 <file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
-  <metadataTypes count="1">
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+  <metadataTypes count="2">
     <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
+    <metadataType name="XLRICHVALUE" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1"/>
   </metadataTypes>
   <futureMetadata name="XLDAPR" count="1">
     <bk>
@@ -52,16 +53,30 @@
       </extLst>
     </bk>
   </futureMetadata>
+  <futureMetadata name="XLRICHVALUE" count="1">
+    <bk>
+      <extLst>
+        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+          <xlrd:rvb i="0"/>
+        </ext>
+      </extLst>
+    </bk>
+  </futureMetadata>
   <cellMetadata count="1">
     <bk>
       <rc t="1" v="0"/>
     </bk>
   </cellMetadata>
+  <valueMetadata count="1">
+    <bk>
+      <rc t="2" v="0"/>
+    </bk>
+  </valueMetadata>
 </metadata>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="783" uniqueCount="256">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="814" uniqueCount="263">
   <si>
     <t>Nome do Filme</t>
   </si>
@@ -829,6 +844,27 @@
   </si>
   <si>
     <t>Total de Horas Assistidas</t>
+  </si>
+  <si>
+    <t>Homem Aranha no Aranha-verso</t>
+  </si>
+  <si>
+    <t>3D-2D</t>
+  </si>
+  <si>
+    <t>A Fuga das Galinhas 2: A Ameaça dos Nuggets</t>
+  </si>
+  <si>
+    <t>ASSISTIDO</t>
+  </si>
+  <si>
+    <t>Nimona</t>
+  </si>
+  <si>
+    <t>Blue Sky Studios</t>
+  </si>
+  <si>
+    <t>Orion e o Escuro</t>
   </si>
 </sst>
 </file>
@@ -840,7 +876,7 @@
     <numFmt numFmtId="165" formatCode="h:mm;@"/>
     <numFmt numFmtId="166" formatCode="_-[$$-409]* #,##0.00_ ;_-[$$-409]* \-#,##0.00\ ;_-[$$-409]* &quot;-&quot;??_ ;_-@_ "/>
     <numFmt numFmtId="167" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
-    <numFmt numFmtId="170" formatCode="[h]:mm:ss;@"/>
+    <numFmt numFmtId="168" formatCode="[h]:mm:ss;@"/>
   </numFmts>
   <fonts count="11" x14ac:knownFonts="1">
     <font>
@@ -1244,7 +1280,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="79">
+  <cellXfs count="80">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1430,6 +1466,12 @@
     <xf numFmtId="167" fontId="3" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="168" fontId="3" fillId="2" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="168" fontId="3" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -1448,17 +1490,266 @@
     <xf numFmtId="0" fontId="10" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="170" fontId="3" fillId="2" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="170" fontId="3" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="17">
+  <dxfs count="35">
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FFC00000"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FFC00000"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FFC00000"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FFC00000"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FFC00000"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="2"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="-0.24994659260841701"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF4444"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF44"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <b/>
@@ -1728,6 +2019,68 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/richData/rdRichValueTypes.xml><?xml version="1.0" encoding="utf-8"?>
+<rvTypesInfo xmlns="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" mc:Ignorable="x">
+  <global>
+    <keyFlags>
+      <key name="_Self">
+        <flag name="ExcludeFromFile" value="1"/>
+        <flag name="ExcludeFromCalcComparison" value="1"/>
+      </key>
+      <key name="_DisplayString">
+        <flag name="ExcludeFromCalcComparison" value="1"/>
+      </key>
+      <key name="_Flags">
+        <flag name="ExcludeFromCalcComparison" value="1"/>
+      </key>
+      <key name="_Format">
+        <flag name="ExcludeFromCalcComparison" value="1"/>
+      </key>
+      <key name="_SubLabel">
+        <flag name="ExcludeFromCalcComparison" value="1"/>
+      </key>
+      <key name="_Attribution">
+        <flag name="ExcludeFromCalcComparison" value="1"/>
+      </key>
+      <key name="_Icon">
+        <flag name="ExcludeFromCalcComparison" value="1"/>
+      </key>
+      <key name="_Display">
+        <flag name="ExcludeFromCalcComparison" value="1"/>
+      </key>
+      <key name="_CanonicalPropertyNames">
+        <flag name="ExcludeFromCalcComparison" value="1"/>
+      </key>
+      <key name="_ClassificationId">
+        <flag name="ExcludeFromCalcComparison" value="1"/>
+      </key>
+    </keyFlags>
+  </global>
+</rvTypesInfo>
+</file>
+
+<file path=xl/richData/rdrichvalue.xml><?xml version="1.0" encoding="utf-8"?>
+<rvData xmlns="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" count="1">
+  <rv s="0">
+    <v>3</v>
+    <v>8</v>
+    <v>41</v>
+    <v>6</v>
+  </rv>
+</rvData>
+</file>
+
+<file path=xl/richData/rdrichvaluestructure.xml><?xml version="1.0" encoding="utf-8"?>
+<rvStructures xmlns="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" count="1">
+  <s t="_error">
+    <k n="colOffset" t="i"/>
+    <k n="errorType" t="i"/>
+    <k n="rwOffset" t="i"/>
+    <k n="subType" t="i"/>
+  </s>
+</rvStructures>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2027,10 +2380,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B5A731FE-9613-428C-993D-C03F78E1A52D}">
-  <dimension ref="A1:AF201"/>
+  <dimension ref="A1:AF218"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="J17" zoomScale="96" zoomScaleNormal="96" workbookViewId="0">
-      <selection activeCell="V31" sqref="V31"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A180" zoomScale="96" zoomScaleNormal="96" workbookViewId="0">
+      <selection activeCell="B206" sqref="B206"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2148,7 +2501,7 @@
         <v>735000000</v>
       </c>
       <c r="K2" s="44">
-        <f>J2-I2</f>
+        <f>IF(OR(ISBLANK(J2),ISBLANK(I2)),"DESCONHECIDO",J2-I2)</f>
         <v>560000000</v>
       </c>
       <c r="L2" s="23">
@@ -2197,7 +2550,7 @@
         <v>406594102</v>
       </c>
       <c r="K3" s="44">
-        <f t="shared" ref="K3:K66" si="3">J3-I3</f>
+        <f t="shared" ref="K3:K66" si="3">IF(OR(ISBLANK(J3),ISBLANK(I3)),"DESCONHECIDO",J3-I3)</f>
         <v>376594102</v>
       </c>
       <c r="L3" s="23">
@@ -2446,18 +2799,9 @@
         <v>4.8611111111111112E-2</v>
       </c>
       <c r="AB6" s="14"/>
-      <c r="AC6" s="9" cm="1">
-        <f t="array" ref="AC6:AF46">_xlfn.CHOOSECOLS(_xlfn._xlws.FILTER($A:$M,($H:$H="Dreamworks")),1,2,13,7)</f>
-        <v>22</v>
-      </c>
-      <c r="AD6" s="11" t="str">
-        <v>Como Treinar o Seu Dragão</v>
-      </c>
-      <c r="AE6" s="9" t="str">
-        <v>ASSISTIDO</v>
-      </c>
-      <c r="AF6" s="64">
-        <v>6.805555555555555E-2</v>
+      <c r="AC6" s="9" t="e" cm="1" vm="1">
+        <f t="array" aca="1" ref="AC6" ca="1">_xlfn.CHOOSECOLS(_xlfn._xlws.FILTER($A:$M,($H:$H="Dreamworks")),1,2,13,7)</f>
+        <v>#VALUE!</v>
       </c>
     </row>
     <row r="7" spans="1:32" ht="19.5" x14ac:dyDescent="0.3">
@@ -2543,18 +2887,7 @@
         <v>5.486111111111111E-2</v>
       </c>
       <c r="AB7" s="14"/>
-      <c r="AC7" s="62">
-        <v>23</v>
-      </c>
-      <c r="AD7" s="11" t="str">
-        <v>Como Treinar o Seu Dragão 2</v>
-      </c>
-      <c r="AE7" s="9" t="str">
-        <v>ASSISTIDO</v>
-      </c>
-      <c r="AF7" s="64">
-        <v>7.2916666666666671E-2</v>
-      </c>
+      <c r="AC7" s="62"/>
     </row>
     <row r="8" spans="1:32" ht="19.5" x14ac:dyDescent="0.3">
       <c r="A8" s="6">
@@ -2639,18 +2972,7 @@
         <v>7.7777777777777779E-2</v>
       </c>
       <c r="AB8" s="14"/>
-      <c r="AC8" s="62">
-        <v>24</v>
-      </c>
-      <c r="AD8" s="11" t="str">
-        <v>Como Treinar o Seu Dragão 3</v>
-      </c>
-      <c r="AE8" s="9" t="str">
-        <v>ASSISTIDO</v>
-      </c>
-      <c r="AF8" s="64">
-        <v>7.2222222222222229E-2</v>
-      </c>
+      <c r="AC8" s="62"/>
     </row>
     <row r="9" spans="1:32" ht="19.5" x14ac:dyDescent="0.3">
       <c r="A9" s="6">
@@ -2735,18 +3057,7 @@
         <v>7.4999999999999997E-2</v>
       </c>
       <c r="AB9" s="14"/>
-      <c r="AC9" s="62">
-        <v>25</v>
-      </c>
-      <c r="AD9" s="11" t="str">
-        <v>Shrek 1</v>
-      </c>
-      <c r="AE9" s="9" t="str">
-        <v>ASSISTIDO</v>
-      </c>
-      <c r="AF9" s="64">
-        <v>6.1805555555555558E-2</v>
-      </c>
+      <c r="AC9" s="62"/>
     </row>
     <row r="10" spans="1:32" ht="19.5" x14ac:dyDescent="0.3">
       <c r="A10" s="6">
@@ -2831,18 +3142,7 @@
         <v>5.9027777777777783E-2</v>
       </c>
       <c r="AB10" s="14"/>
-      <c r="AC10" s="62">
-        <v>26</v>
-      </c>
-      <c r="AD10" s="11" t="str">
-        <v>Shrek 2</v>
-      </c>
-      <c r="AE10" s="9" t="str">
-        <v>ASSISTIDO</v>
-      </c>
-      <c r="AF10" s="64">
-        <v>7.2916666666666671E-2</v>
-      </c>
+      <c r="AC10" s="62"/>
     </row>
     <row r="11" spans="1:32" ht="19.5" x14ac:dyDescent="0.3">
       <c r="A11" s="6">
@@ -2927,18 +3227,7 @@
         <v>5.7638888888888885E-2</v>
       </c>
       <c r="AB11" s="14"/>
-      <c r="AC11" s="62">
-        <v>27</v>
-      </c>
-      <c r="AD11" s="11" t="str">
-        <v>Shrek 3</v>
-      </c>
-      <c r="AE11" s="9" t="str">
-        <v>ASSISTIDO</v>
-      </c>
-      <c r="AF11" s="64">
-        <v>6.458333333333334E-2</v>
-      </c>
+      <c r="AC11" s="62"/>
     </row>
     <row r="12" spans="1:32" ht="19.5" x14ac:dyDescent="0.3">
       <c r="A12" s="6">
@@ -3023,18 +3312,7 @@
         <v>7.2222222222222229E-2</v>
       </c>
       <c r="AB12" s="14"/>
-      <c r="AC12" s="62">
-        <v>28</v>
-      </c>
-      <c r="AD12" s="11" t="str">
-        <v>Spirit: O Corcéu Indomável</v>
-      </c>
-      <c r="AE12" s="9" t="str">
-        <v>ASSISTIDO</v>
-      </c>
-      <c r="AF12" s="64">
-        <v>5.8333333333333327E-2</v>
-      </c>
+      <c r="AC12" s="62"/>
     </row>
     <row r="13" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A13" s="6">
@@ -3114,18 +3392,7 @@
         <v>7.5694444444444439E-2</v>
       </c>
       <c r="AB13" s="14"/>
-      <c r="AC13" s="62">
-        <v>29</v>
-      </c>
-      <c r="AD13" s="11" t="str">
-        <v>O Caminho Para El Dorado</v>
-      </c>
-      <c r="AE13" s="9" t="str">
-        <v>ASSISTIDO</v>
-      </c>
-      <c r="AF13" s="64">
-        <v>6.1805555555555558E-2</v>
-      </c>
+      <c r="AC13" s="62"/>
     </row>
     <row r="14" spans="1:32" ht="19.5" x14ac:dyDescent="0.3">
       <c r="A14" s="6">
@@ -3207,18 +3474,7 @@
         <v>6.9444444444444434E-2</v>
       </c>
       <c r="AB14" s="14"/>
-      <c r="AC14" s="62">
-        <v>33</v>
-      </c>
-      <c r="AD14" s="11" t="str">
-        <v>Kung Fu Panda</v>
-      </c>
-      <c r="AE14" s="9" t="str">
-        <v>ASSISTIDO</v>
-      </c>
-      <c r="AF14" s="64">
-        <v>6.3888888888888884E-2</v>
-      </c>
+      <c r="AC14" s="62"/>
     </row>
     <row r="15" spans="1:32" ht="19.5" x14ac:dyDescent="0.3">
       <c r="A15" s="6">
@@ -3302,18 +3558,7 @@
         <v>7.4305555555555555E-2</v>
       </c>
       <c r="AB15" s="14"/>
-      <c r="AC15" s="62">
-        <v>34</v>
-      </c>
-      <c r="AD15" s="11" t="str">
-        <v>Kung Fu Panda 2</v>
-      </c>
-      <c r="AE15" s="9" t="str">
-        <v>ASSISTIDO</v>
-      </c>
-      <c r="AF15" s="64">
-        <v>6.3888888888888884E-2</v>
-      </c>
+      <c r="AC15" s="62"/>
     </row>
     <row r="16" spans="1:32" ht="19.5" x14ac:dyDescent="0.3">
       <c r="A16" s="6">
@@ -3398,20 +3643,9 @@
         <v>7.4999999999999997E-2</v>
       </c>
       <c r="AB16" s="14"/>
-      <c r="AC16" s="62">
-        <v>35</v>
-      </c>
-      <c r="AD16" s="11" t="str">
-        <v>Kung Fu Panda 3</v>
-      </c>
-      <c r="AE16" s="9" t="str">
-        <v>ASSISTIDO</v>
-      </c>
-      <c r="AF16" s="64">
-        <v>6.5972222222222224E-2</v>
-      </c>
-    </row>
-    <row r="17" spans="1:32" ht="19.5" x14ac:dyDescent="0.3">
+      <c r="AC16" s="62"/>
+    </row>
+    <row r="17" spans="1:29" ht="19.5" x14ac:dyDescent="0.3">
       <c r="A17" s="6">
         <f t="shared" si="2"/>
         <v>16</v>
@@ -3494,20 +3728,9 @@
         <v>7.9861111111111105E-2</v>
       </c>
       <c r="AB17" s="14"/>
-      <c r="AC17" s="62">
-        <v>36</v>
-      </c>
-      <c r="AD17" s="11" t="str">
-        <v>A Origem dos Guardiões</v>
-      </c>
-      <c r="AE17" s="9" t="str">
-        <v>ASSISTIDO</v>
-      </c>
-      <c r="AF17" s="64">
-        <v>6.7361111111111108E-2</v>
-      </c>
-    </row>
-    <row r="18" spans="1:32" ht="19.5" x14ac:dyDescent="0.3">
+      <c r="AC17" s="62"/>
+    </row>
+    <row r="18" spans="1:29" ht="19.5" x14ac:dyDescent="0.3">
       <c r="A18" s="6">
         <f t="shared" si="2"/>
         <v>17</v>
@@ -3590,20 +3813,9 @@
         <v>7.4999999999999997E-2</v>
       </c>
       <c r="AB18" s="14"/>
-      <c r="AC18" s="62">
-        <v>37</v>
-      </c>
-      <c r="AD18" s="11" t="str">
-        <v>O Gato De Botas</v>
-      </c>
-      <c r="AE18" s="9" t="str">
-        <v>ASSISTIDO</v>
-      </c>
-      <c r="AF18" s="64">
-        <v>6.25E-2</v>
-      </c>
-    </row>
-    <row r="19" spans="1:32" ht="19.5" x14ac:dyDescent="0.3">
+      <c r="AC18" s="62"/>
+    </row>
+    <row r="19" spans="1:29" ht="19.5" x14ac:dyDescent="0.3">
       <c r="A19" s="6">
         <f t="shared" si="2"/>
         <v>18</v>
@@ -3686,20 +3898,9 @@
         <v>5.9027777777777783E-2</v>
       </c>
       <c r="AB19" s="14"/>
-      <c r="AC19" s="62">
-        <v>101</v>
-      </c>
-      <c r="AD19" s="11" t="str">
-        <v>Madagascar</v>
-      </c>
-      <c r="AE19" s="9" t="str">
-        <v>ASSISTIDO</v>
-      </c>
-      <c r="AF19" s="64">
-        <v>5.9722222222222225E-2</v>
-      </c>
-    </row>
-    <row r="20" spans="1:32" ht="19.5" x14ac:dyDescent="0.3">
+      <c r="AC19" s="62"/>
+    </row>
+    <row r="20" spans="1:29" ht="19.5" x14ac:dyDescent="0.3">
       <c r="A20" s="6">
         <f t="shared" si="2"/>
         <v>19</v>
@@ -3782,20 +3983,9 @@
         <v>6.5972222222222224E-2</v>
       </c>
       <c r="AB20" s="14"/>
-      <c r="AC20" s="62">
-        <v>118</v>
-      </c>
-      <c r="AD20" s="11" t="str">
-        <v>Gato de Botas 2: O Último Pedido</v>
-      </c>
-      <c r="AE20" s="9" t="str">
-        <v>ASSISTIDO</v>
-      </c>
-      <c r="AF20" s="64">
-        <v>7.0833333333333331E-2</v>
-      </c>
-    </row>
-    <row r="21" spans="1:32" ht="19.5" x14ac:dyDescent="0.3">
+      <c r="AC20" s="62"/>
+    </row>
+    <row r="21" spans="1:29" ht="19.5" x14ac:dyDescent="0.3">
       <c r="A21" s="6">
         <f t="shared" si="2"/>
         <v>20</v>
@@ -3877,20 +4067,9 @@
         <v>5.2777777777777778E-2</v>
       </c>
       <c r="AB21" s="14"/>
-      <c r="AC21" s="62">
-        <v>122</v>
-      </c>
-      <c r="AD21" s="11" t="str">
-        <v>Sinbad: A Lenda dos sete mares</v>
-      </c>
-      <c r="AE21" s="9" t="str">
-        <v>NÃO ASSISTIDO</v>
-      </c>
-      <c r="AF21" s="64">
-        <v>5.9722222222222225E-2</v>
-      </c>
-    </row>
-    <row r="22" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="AC21" s="62"/>
+    </row>
+    <row r="22" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A22" s="6">
         <f t="shared" si="2"/>
         <v>21</v>
@@ -3965,20 +4144,9 @@
         <v>5.2083333333333336E-2</v>
       </c>
       <c r="AB22" s="14"/>
-      <c r="AC22" s="62">
-        <v>136</v>
-      </c>
-      <c r="AD22" s="11" t="str">
-        <v>O Príncipe do Egito</v>
-      </c>
-      <c r="AE22" s="9" t="str">
-        <v>NÃO ASSISTIDO</v>
-      </c>
-      <c r="AF22" s="64">
-        <v>6.8749999999999992E-2</v>
-      </c>
-    </row>
-    <row r="23" spans="1:32" ht="19.5" x14ac:dyDescent="0.3">
+      <c r="AC22" s="62"/>
+    </row>
+    <row r="23" spans="1:29" ht="19.5" x14ac:dyDescent="0.3">
       <c r="A23" s="6">
         <f t="shared" si="2"/>
         <v>22</v>
@@ -4057,20 +4225,8 @@
         <v>7.0833333333333331E-2</v>
       </c>
       <c r="AB23" s="14"/>
-      <c r="AC23" s="9">
-        <v>177</v>
-      </c>
-      <c r="AD23" s="11" t="str">
-        <v>FormiguinhaZ</v>
-      </c>
-      <c r="AE23" s="9" t="str">
-        <v>NÃO ASSISTIDO</v>
-      </c>
-      <c r="AF23" s="64">
-        <v>5.7638888888888885E-2</v>
-      </c>
-    </row>
-    <row r="24" spans="1:32" ht="19.5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="24" spans="1:29" ht="19.5" x14ac:dyDescent="0.3">
       <c r="A24" s="6">
         <f t="shared" si="2"/>
         <v>23</v>
@@ -4151,20 +4307,8 @@
         <v>6.1111111111111116E-2</v>
       </c>
       <c r="AB24" s="14"/>
-      <c r="AC24" s="9">
-        <v>178</v>
-      </c>
-      <c r="AD24" s="11" t="str">
-        <v>O Espanta Tubarões</v>
-      </c>
-      <c r="AE24" s="9" t="str">
-        <v>NÃO ASSISTIDO</v>
-      </c>
-      <c r="AF24" s="64">
-        <v>6.25E-2</v>
-      </c>
-    </row>
-    <row r="25" spans="1:32" ht="19.5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="25" spans="1:29" ht="19.5" x14ac:dyDescent="0.3">
       <c r="A25" s="6">
         <f t="shared" si="2"/>
         <v>24</v>
@@ -4246,20 +4390,8 @@
         <v>6.0416666666666667E-2</v>
       </c>
       <c r="AB25" s="14"/>
-      <c r="AC25" s="9">
-        <v>179</v>
-      </c>
-      <c r="AD25" s="11" t="str">
-        <v>Wallace &amp; Gromit: A Batalha dos vegetais</v>
-      </c>
-      <c r="AE25" s="9" t="str">
-        <v>ASSISTIDO</v>
-      </c>
-      <c r="AF25" s="64">
-        <v>5.9027777777777783E-2</v>
-      </c>
-    </row>
-    <row r="26" spans="1:32" ht="19.5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="26" spans="1:29" ht="19.5" x14ac:dyDescent="0.3">
       <c r="A26" s="6">
         <f t="shared" si="2"/>
         <v>25</v>
@@ -4341,20 +4473,8 @@
         <v>5.6250000000000001E-2</v>
       </c>
       <c r="AB26" s="14"/>
-      <c r="AC26" s="9">
-        <v>180</v>
-      </c>
-      <c r="AD26" s="11" t="str">
-        <v>Os Sem Floresta</v>
-      </c>
-      <c r="AE26" s="9" t="str">
-        <v>NÃO ASSISTIDO</v>
-      </c>
-      <c r="AF26" s="64">
-        <v>6.0416666666666667E-2</v>
-      </c>
-    </row>
-    <row r="27" spans="1:32" ht="19.5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="27" spans="1:29" ht="19.5" x14ac:dyDescent="0.3">
       <c r="A27" s="6">
         <f t="shared" si="2"/>
         <v>26</v>
@@ -4436,20 +4556,8 @@
         <v>6.25E-2</v>
       </c>
       <c r="AB27" s="14"/>
-      <c r="AC27" s="9">
-        <v>181</v>
-      </c>
-      <c r="AD27" s="11" t="str">
-        <v>Por Água Abaixo</v>
-      </c>
-      <c r="AE27" s="9" t="str">
-        <v>NÃO ASSISTIDO</v>
-      </c>
-      <c r="AF27" s="64">
-        <v>5.9722222222222225E-2</v>
-      </c>
-    </row>
-    <row r="28" spans="1:32" x14ac:dyDescent="0.25">
+    </row>
+    <row r="28" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A28" s="6">
         <f t="shared" si="2"/>
         <v>27</v>
@@ -4524,20 +4632,8 @@
         <v>6.458333333333334E-2</v>
       </c>
       <c r="AB28" s="14"/>
-      <c r="AC28" s="9">
-        <v>182</v>
-      </c>
-      <c r="AD28" s="11" t="str">
-        <v>Bee Movie: A História de uma Abelha</v>
-      </c>
-      <c r="AE28" s="9" t="str">
-        <v>NÃO ASSISTIDO</v>
-      </c>
-      <c r="AF28" s="64">
-        <v>6.3194444444444442E-2</v>
-      </c>
-    </row>
-    <row r="29" spans="1:32" ht="19.5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="29" spans="1:29" ht="19.5" x14ac:dyDescent="0.3">
       <c r="A29" s="6">
         <f t="shared" si="2"/>
         <v>28</v>
@@ -4616,20 +4712,8 @@
         <v>5.8333333333333327E-2</v>
       </c>
       <c r="AB29" s="14"/>
-      <c r="AC29" s="9">
-        <v>183</v>
-      </c>
-      <c r="AD29" s="11" t="str">
-        <v>Madagascar 2: A Grande Escapada</v>
-      </c>
-      <c r="AE29" s="9" t="str">
-        <v>ASSISTIDO</v>
-      </c>
-      <c r="AF29" s="64">
-        <v>6.1805555555555558E-2</v>
-      </c>
-    </row>
-    <row r="30" spans="1:32" ht="19.5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="30" spans="1:29" ht="19.5" x14ac:dyDescent="0.3">
       <c r="A30" s="6">
         <f t="shared" si="2"/>
         <v>29</v>
@@ -4682,7 +4766,7 @@
       </c>
       <c r="Q30" s="19">
         <f>COUNTIF(M:M,"ASSISTIDO")</f>
-        <v>148</v>
+        <v>165</v>
       </c>
       <c r="R30" s="26"/>
       <c r="S30" s="40">
@@ -4711,20 +4795,8 @@
         <v>6.3194444444444442E-2</v>
       </c>
       <c r="AB30" s="14"/>
-      <c r="AC30" s="9">
-        <v>184</v>
-      </c>
-      <c r="AD30" s="11" t="str">
-        <v>Monstros Vs Aliens</v>
-      </c>
-      <c r="AE30" s="9" t="str">
-        <v>NÃO ASSISTIDO</v>
-      </c>
-      <c r="AF30" s="64">
-        <v>7.0833333333333331E-2</v>
-      </c>
-    </row>
-    <row r="31" spans="1:32" ht="19.5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="31" spans="1:29" ht="19.5" x14ac:dyDescent="0.3">
       <c r="A31" s="6">
         <f t="shared" si="2"/>
         <v>30</v>
@@ -4780,12 +4852,12 @@
         <v>52</v>
       </c>
       <c r="R31" s="26"/>
-      <c r="S31" s="71" t="s">
+      <c r="S31" s="73" t="s">
         <v>206</v>
       </c>
-      <c r="T31" s="72"/>
-      <c r="U31" s="73"/>
-      <c r="V31" s="77">
+      <c r="T31" s="74"/>
+      <c r="U31" s="75"/>
+      <c r="V31" s="71">
         <f ca="1">SUMIF($U$6:$V$30,"ASSISTIDO",$V$6:$V$30)</f>
         <v>1.5416666666666667</v>
       </c>
@@ -4803,20 +4875,8 @@
         <v>6.1805555555555558E-2</v>
       </c>
       <c r="AB31" s="14"/>
-      <c r="AC31" s="9">
-        <v>185</v>
-      </c>
-      <c r="AD31" s="11" t="str">
-        <v>Shrek Para Sempre</v>
-      </c>
-      <c r="AE31" s="9" t="str">
-        <v>NÃO ASSISTIDO</v>
-      </c>
-      <c r="AF31" s="64">
-        <v>6.458333333333334E-2</v>
-      </c>
-    </row>
-    <row r="32" spans="1:32" ht="19.5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="32" spans="1:29" ht="19.5" x14ac:dyDescent="0.3">
       <c r="A32" s="6">
         <f t="shared" si="2"/>
         <v>31</v>
@@ -4869,7 +4929,7 @@
       </c>
       <c r="Q32" s="20">
         <f>MAX(A:A)</f>
-        <v>200</v>
+        <v>217</v>
       </c>
       <c r="S32" s="37"/>
       <c r="T32" s="37"/>
@@ -4889,18 +4949,6 @@
         <v>5.7638888888888885E-2</v>
       </c>
       <c r="AB32" s="14"/>
-      <c r="AC32" s="9">
-        <v>186</v>
-      </c>
-      <c r="AD32" s="11" t="str">
-        <v>Megamente</v>
-      </c>
-      <c r="AE32" s="9" t="str">
-        <v>NÃO ASSISTIDO</v>
-      </c>
-      <c r="AF32" s="64">
-        <v>6.6666666666666666E-2</v>
-      </c>
     </row>
     <row r="33" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A33" s="6">
@@ -4964,18 +5012,6 @@
         <v>6.7361111111111108E-2</v>
       </c>
       <c r="AB33" s="14"/>
-      <c r="AC33" s="9">
-        <v>187</v>
-      </c>
-      <c r="AD33" s="11" t="str">
-        <v>Madagascar 3: Os Procurados</v>
-      </c>
-      <c r="AE33" s="9" t="str">
-        <v>ASSISTIDO</v>
-      </c>
-      <c r="AF33" s="64">
-        <v>6.5972222222222224E-2</v>
-      </c>
     </row>
     <row r="34" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A34" s="6">
@@ -5039,18 +5075,6 @@
         <v>6.1111111111111116E-2</v>
       </c>
       <c r="AB34" s="14"/>
-      <c r="AC34" s="9">
-        <v>188</v>
-      </c>
-      <c r="AD34" s="11" t="str">
-        <v>Turbo</v>
-      </c>
-      <c r="AE34" s="9" t="str">
-        <v>NÃO ASSISTIDO</v>
-      </c>
-      <c r="AF34" s="64">
-        <v>6.6666666666666666E-2</v>
-      </c>
     </row>
     <row r="35" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A35" s="6">
@@ -5114,18 +5138,6 @@
         <v>9.930555555555555E-2</v>
       </c>
       <c r="AB35" s="14"/>
-      <c r="AC35" s="9">
-        <v>189</v>
-      </c>
-      <c r="AD35" s="11" t="str">
-        <v>As Aventuras de Peabody &amp; Sherman</v>
-      </c>
-      <c r="AE35" s="9" t="str">
-        <v>NÃO ASSISTIDO</v>
-      </c>
-      <c r="AF35" s="64">
-        <v>6.3888888888888884E-2</v>
-      </c>
     </row>
     <row r="36" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A36" s="6">
@@ -5189,18 +5201,6 @@
         <v>0.10486111111111111</v>
       </c>
       <c r="AB36" s="14"/>
-      <c r="AC36" s="9">
-        <v>190</v>
-      </c>
-      <c r="AD36" s="11" t="str">
-        <v>Os Pinguins de Madagascar</v>
-      </c>
-      <c r="AE36" s="9" t="str">
-        <v>NÃO ASSISTIDO</v>
-      </c>
-      <c r="AF36" s="64">
-        <v>6.3888888888888884E-2</v>
-      </c>
     </row>
     <row r="37" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A37" s="6">
@@ -5264,18 +5264,6 @@
         <v>0.11666666666666665</v>
       </c>
       <c r="AB37" s="14"/>
-      <c r="AC37" s="9">
-        <v>191</v>
-      </c>
-      <c r="AD37" s="11" t="str">
-        <v>Cada um na sua casa</v>
-      </c>
-      <c r="AE37" s="9" t="str">
-        <v>NÃO ASSISTIDO</v>
-      </c>
-      <c r="AF37" s="64">
-        <v>6.5277777777777782E-2</v>
-      </c>
     </row>
     <row r="38" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A38" s="6">
@@ -5339,18 +5327,6 @@
         <v>9.7916666666666666E-2</v>
       </c>
       <c r="AB38" s="14"/>
-      <c r="AC38" s="9">
-        <v>192</v>
-      </c>
-      <c r="AD38" s="11" t="str">
-        <v>Trolls</v>
-      </c>
-      <c r="AE38" s="9" t="str">
-        <v>NÃO ASSISTIDO</v>
-      </c>
-      <c r="AF38" s="64">
-        <v>6.458333333333334E-2</v>
-      </c>
     </row>
     <row r="39" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A39" s="6">
@@ -5414,18 +5390,6 @@
         <v>8.9583333333333334E-2</v>
       </c>
       <c r="AB39" s="14"/>
-      <c r="AC39" s="9">
-        <v>193</v>
-      </c>
-      <c r="AD39" s="11" t="str">
-        <v>O Poderoso Chefinho</v>
-      </c>
-      <c r="AE39" s="9" t="str">
-        <v>NÃO ASSISTIDO</v>
-      </c>
-      <c r="AF39" s="64">
-        <v>6.7361111111111108E-2</v>
-      </c>
     </row>
     <row r="40" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A40" s="6">
@@ -5489,18 +5453,6 @@
         <v>5.6250000000000001E-2</v>
       </c>
       <c r="AB40" s="14"/>
-      <c r="AC40" s="9">
-        <v>194</v>
-      </c>
-      <c r="AD40" s="11" t="str">
-        <v>As Aventuras do Capitão Cueca</v>
-      </c>
-      <c r="AE40" s="9" t="str">
-        <v>NÃO ASSISTIDO</v>
-      </c>
-      <c r="AF40" s="64">
-        <v>6.1805555555555558E-2</v>
-      </c>
     </row>
     <row r="41" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A41" s="6">
@@ -5564,18 +5516,6 @@
         <v>5.1388888888888894E-2</v>
       </c>
       <c r="AB41" s="14"/>
-      <c r="AC41" s="9">
-        <v>195</v>
-      </c>
-      <c r="AD41" s="11" t="str">
-        <v>Abominável</v>
-      </c>
-      <c r="AE41" s="9" t="str">
-        <v>NÃO ASSISTIDO</v>
-      </c>
-      <c r="AF41" s="64">
-        <v>6.3888888888888884E-2</v>
-      </c>
     </row>
     <row r="42" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A42" s="6">
@@ -5639,18 +5579,6 @@
         <v>5.4166666666666669E-2</v>
       </c>
       <c r="AB42" s="14"/>
-      <c r="AC42" s="9">
-        <v>196</v>
-      </c>
-      <c r="AD42" s="11" t="str">
-        <v>Trolls 2</v>
-      </c>
-      <c r="AE42" s="9" t="str">
-        <v>NÃO ASSISTIDO</v>
-      </c>
-      <c r="AF42" s="64">
-        <v>6.3194444444444442E-2</v>
-      </c>
     </row>
     <row r="43" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A43" s="6">
@@ -5714,18 +5642,6 @@
         <v>5.1388888888888894E-2</v>
       </c>
       <c r="AB43" s="14"/>
-      <c r="AC43" s="9">
-        <v>197</v>
-      </c>
-      <c r="AD43" s="11" t="str">
-        <v>Os Croods</v>
-      </c>
-      <c r="AE43" s="9" t="str">
-        <v>NÃO ASSISTIDO</v>
-      </c>
-      <c r="AF43" s="64">
-        <v>6.805555555555555E-2</v>
-      </c>
     </row>
     <row r="44" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A44" s="6">
@@ -5789,18 +5705,6 @@
         <v>5.2777777777777778E-2</v>
       </c>
       <c r="AB44" s="14"/>
-      <c r="AC44" s="9">
-        <v>198</v>
-      </c>
-      <c r="AD44" s="11" t="str">
-        <v>Os Croods 2: Uma Nova Era</v>
-      </c>
-      <c r="AE44" s="9" t="str">
-        <v>NÃO ASSISTIDO</v>
-      </c>
-      <c r="AF44" s="64">
-        <v>6.5972222222222224E-2</v>
-      </c>
     </row>
     <row r="45" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A45" s="6">
@@ -5864,18 +5768,6 @@
         <v>5.2777777777777778E-2</v>
       </c>
       <c r="AB45" s="14"/>
-      <c r="AC45" s="9">
-        <v>199</v>
-      </c>
-      <c r="AD45" s="11" t="str">
-        <v>Spirit: O Indomável</v>
-      </c>
-      <c r="AE45" s="9" t="str">
-        <v>NÃO ASSISTIDO</v>
-      </c>
-      <c r="AF45" s="64">
-        <v>6.1111111111111116E-2</v>
-      </c>
     </row>
     <row r="46" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A46" s="6">
@@ -5939,18 +5831,6 @@
         <v>5.4166666666666669E-2</v>
       </c>
       <c r="AB46" s="14"/>
-      <c r="AC46" s="9">
-        <v>200</v>
-      </c>
-      <c r="AD46" s="11" t="str">
-        <v>O Poderoso Chefinho 2: Negócios de Família</v>
-      </c>
-      <c r="AE46" s="9" t="str">
-        <v>NÃO ASSISTIDO</v>
-      </c>
-      <c r="AF46" s="64">
-        <v>7.4305555555555555E-2</v>
-      </c>
     </row>
     <row r="47" spans="1:32" ht="19.5" x14ac:dyDescent="0.25">
       <c r="A47" s="6">
@@ -6014,14 +5894,14 @@
         <v>5.4166666666666669E-2</v>
       </c>
       <c r="AB47" s="14"/>
-      <c r="AC47" s="74" t="s">
+      <c r="AC47" s="76" t="s">
         <v>255</v>
       </c>
-      <c r="AD47" s="75"/>
-      <c r="AE47" s="76"/>
-      <c r="AF47" s="78">
+      <c r="AD47" s="77"/>
+      <c r="AE47" s="78"/>
+      <c r="AF47" s="72">
         <f>SUMIF($AE$6:$AE$46,"ASSISTIDO",$AF$6:$AF$46)</f>
-        <v>1.1736111111111112</v>
+        <v>0</v>
       </c>
     </row>
     <row r="48" spans="1:32" x14ac:dyDescent="0.25">
@@ -7236,7 +7116,7 @@
         <v>0</v>
       </c>
       <c r="K67" s="44">
-        <f t="shared" ref="K67:K130" si="10">J67-I67</f>
+        <f t="shared" ref="K67:K130" si="10">IF(OR(ISBLANK(J67),ISBLANK(I67)),"DESCONHECIDO",J67-I67)</f>
         <v>0</v>
       </c>
       <c r="L67" s="23">
@@ -7800,12 +7680,12 @@
         <f t="shared" si="11"/>
         <v>75</v>
       </c>
-      <c r="X76" s="71" t="s">
+      <c r="X76" s="73" t="s">
         <v>206</v>
       </c>
-      <c r="Y76" s="72"/>
-      <c r="Z76" s="73"/>
-      <c r="AA76" s="77">
+      <c r="Y76" s="74"/>
+      <c r="Z76" s="75"/>
+      <c r="AA76" s="71">
         <f>SUMIF($Z$6:$Z$75,"ASSISTIDO",$AA$6:$AA$75)</f>
         <v>3.098611111111111</v>
       </c>
@@ -10444,7 +10324,7 @@
         <v>462000000</v>
       </c>
       <c r="K131" s="44">
-        <f t="shared" ref="K131:K177" si="17">J131-I131</f>
+        <f t="shared" ref="K131:K194" si="17">IF(OR(ISBLANK(J131),ISBLANK(I131)),"DESCONHECIDO",J131-I131)</f>
         <v>342000000</v>
       </c>
       <c r="L131" s="23">
@@ -11458,7 +11338,7 @@
         <v>ASSISTIDO</v>
       </c>
       <c r="N152" s="6">
-        <f t="shared" ref="N152:N201" si="23">ROW()-1</f>
+        <f t="shared" ref="N152:N215" si="23">ROW()-1</f>
         <v>151</v>
       </c>
     </row>
@@ -12594,14 +12474,14 @@
         <v>171800000</v>
       </c>
       <c r="K178" s="44">
-        <f t="shared" ref="K178:K189" si="30">J178-I178</f>
+        <f t="shared" si="17"/>
         <v>66800000</v>
       </c>
       <c r="L178" s="23">
         <v>0</v>
       </c>
       <c r="M178" s="25" t="str">
-        <f t="shared" ref="M178:M189" si="31">IF(ISBLANK(F178),"NÃO ASSISTIDO","ASSISTIDO")</f>
+        <f t="shared" ref="M178:M189" si="30">IF(ISBLANK(F178),"NÃO ASSISTIDO","ASSISTIDO")</f>
         <v>NÃO ASSISTIDO</v>
       </c>
       <c r="N178" s="6">
@@ -12637,14 +12517,14 @@
         <v>374600000</v>
       </c>
       <c r="K179" s="44">
+        <f t="shared" si="17"/>
+        <v>299600000</v>
+      </c>
+      <c r="L179" s="23">
+        <v>0</v>
+      </c>
+      <c r="M179" s="25" t="str">
         <f t="shared" si="30"/>
-        <v>299600000</v>
-      </c>
-      <c r="L179" s="23">
-        <v>0</v>
-      </c>
-      <c r="M179" s="25" t="str">
-        <f t="shared" si="31"/>
         <v>NÃO ASSISTIDO</v>
       </c>
       <c r="N179" s="6">
@@ -12685,14 +12565,14 @@
         <v>192600000</v>
       </c>
       <c r="K180" s="44">
+        <f t="shared" si="17"/>
+        <v>162600000</v>
+      </c>
+      <c r="L180" s="23">
+        <v>0</v>
+      </c>
+      <c r="M180" s="25" t="str">
         <f t="shared" si="30"/>
-        <v>162600000</v>
-      </c>
-      <c r="L180" s="23">
-        <v>0</v>
-      </c>
-      <c r="M180" s="25" t="str">
-        <f t="shared" si="31"/>
         <v>ASSISTIDO</v>
       </c>
       <c r="N180" s="6">
@@ -12728,14 +12608,14 @@
         <v>336002996</v>
       </c>
       <c r="K181" s="44">
+        <f t="shared" si="17"/>
+        <v>256002996</v>
+      </c>
+      <c r="L181" s="23">
+        <v>0</v>
+      </c>
+      <c r="M181" s="25" t="str">
         <f t="shared" si="30"/>
-        <v>256002996</v>
-      </c>
-      <c r="L181" s="23">
-        <v>0</v>
-      </c>
-      <c r="M181" s="25" t="str">
-        <f t="shared" si="31"/>
         <v>NÃO ASSISTIDO</v>
       </c>
       <c r="N181" s="6">
@@ -12771,14 +12651,14 @@
         <v>178000000</v>
       </c>
       <c r="K182" s="44">
+        <f t="shared" si="17"/>
+        <v>29000000</v>
+      </c>
+      <c r="L182" s="23">
+        <v>0</v>
+      </c>
+      <c r="M182" s="25" t="str">
         <f t="shared" si="30"/>
-        <v>29000000</v>
-      </c>
-      <c r="L182" s="23">
-        <v>0</v>
-      </c>
-      <c r="M182" s="25" t="str">
-        <f t="shared" si="31"/>
         <v>NÃO ASSISTIDO</v>
       </c>
       <c r="N182" s="6">
@@ -12814,14 +12694,14 @@
         <v>293500000</v>
       </c>
       <c r="K183" s="44">
+        <f t="shared" si="17"/>
+        <v>143500000</v>
+      </c>
+      <c r="L183" s="23">
+        <v>0</v>
+      </c>
+      <c r="M183" s="25" t="str">
         <f t="shared" si="30"/>
-        <v>143500000</v>
-      </c>
-      <c r="L183" s="23">
-        <v>0</v>
-      </c>
-      <c r="M183" s="25" t="str">
-        <f t="shared" si="31"/>
         <v>NÃO ASSISTIDO</v>
       </c>
       <c r="N183" s="6">
@@ -12862,14 +12742,14 @@
         <v>603900000</v>
       </c>
       <c r="K184" s="44">
+        <f t="shared" si="17"/>
+        <v>453900000</v>
+      </c>
+      <c r="L184" s="23">
+        <v>0</v>
+      </c>
+      <c r="M184" s="25" t="str">
         <f t="shared" si="30"/>
-        <v>453900000</v>
-      </c>
-      <c r="L184" s="23">
-        <v>0</v>
-      </c>
-      <c r="M184" s="25" t="str">
-        <f t="shared" si="31"/>
         <v>ASSISTIDO</v>
       </c>
       <c r="N184" s="6">
@@ -12905,14 +12785,14 @@
         <v>381700000</v>
       </c>
       <c r="K185" s="44">
+        <f t="shared" si="17"/>
+        <v>206700000</v>
+      </c>
+      <c r="L185" s="23">
+        <v>0</v>
+      </c>
+      <c r="M185" s="25" t="str">
         <f t="shared" si="30"/>
-        <v>206700000</v>
-      </c>
-      <c r="L185" s="23">
-        <v>0</v>
-      </c>
-      <c r="M185" s="25" t="str">
-        <f t="shared" si="31"/>
         <v>NÃO ASSISTIDO</v>
       </c>
       <c r="N185" s="6">
@@ -12948,14 +12828,14 @@
         <v>756200000</v>
       </c>
       <c r="K186" s="44">
+        <f t="shared" si="17"/>
+        <v>621200000</v>
+      </c>
+      <c r="L186" s="23">
+        <v>0</v>
+      </c>
+      <c r="M186" s="25" t="str">
         <f t="shared" si="30"/>
-        <v>621200000</v>
-      </c>
-      <c r="L186" s="23">
-        <v>0</v>
-      </c>
-      <c r="M186" s="25" t="str">
-        <f t="shared" si="31"/>
         <v>NÃO ASSISTIDO</v>
       </c>
       <c r="N186" s="6">
@@ -12991,14 +12871,14 @@
         <v>321900000</v>
       </c>
       <c r="K187" s="44">
+        <f t="shared" si="17"/>
+        <v>191900000</v>
+      </c>
+      <c r="L187" s="23">
+        <v>0</v>
+      </c>
+      <c r="M187" s="25" t="str">
         <f t="shared" si="30"/>
-        <v>191900000</v>
-      </c>
-      <c r="L187" s="23">
-        <v>0</v>
-      </c>
-      <c r="M187" s="25" t="str">
-        <f t="shared" si="31"/>
         <v>NÃO ASSISTIDO</v>
       </c>
       <c r="N187" s="6">
@@ -13039,14 +12919,14 @@
         <v>746000000</v>
       </c>
       <c r="K188" s="44">
+        <f t="shared" si="17"/>
+        <v>601000000</v>
+      </c>
+      <c r="L188" s="23">
+        <v>0</v>
+      </c>
+      <c r="M188" s="25" t="str">
         <f t="shared" si="30"/>
-        <v>601000000</v>
-      </c>
-      <c r="L188" s="23">
-        <v>0</v>
-      </c>
-      <c r="M188" s="25" t="str">
-        <f t="shared" si="31"/>
         <v>ASSISTIDO</v>
       </c>
       <c r="N188" s="6">
@@ -13082,14 +12962,14 @@
         <v>282600000</v>
       </c>
       <c r="K189" s="44">
+        <f t="shared" si="17"/>
+        <v>155600000</v>
+      </c>
+      <c r="L189" s="23">
+        <v>0</v>
+      </c>
+      <c r="M189" s="25" t="str">
         <f t="shared" si="30"/>
-        <v>155600000</v>
-      </c>
-      <c r="L189" s="23">
-        <v>0</v>
-      </c>
-      <c r="M189" s="25" t="str">
-        <f t="shared" si="31"/>
         <v>NÃO ASSISTIDO</v>
       </c>
       <c r="N189" s="6">
@@ -13125,14 +13005,14 @@
         <v>260800000</v>
       </c>
       <c r="K190" s="44">
-        <f t="shared" ref="K190:K198" si="32">J190-I190</f>
+        <f t="shared" si="17"/>
         <v>115800000</v>
       </c>
       <c r="L190" s="23">
         <v>0</v>
       </c>
       <c r="M190" s="25" t="str">
-        <f t="shared" ref="M190:M198" si="33">IF(ISBLANK(F190),"NÃO ASSISTIDO","ASSISTIDO")</f>
+        <f t="shared" ref="M190:M198" si="31">IF(ISBLANK(F190),"NÃO ASSISTIDO","ASSISTIDO")</f>
         <v>NÃO ASSISTIDO</v>
       </c>
       <c r="N190" s="6">
@@ -13168,14 +13048,14 @@
         <v>373500000</v>
       </c>
       <c r="K191" s="44">
-        <f t="shared" si="32"/>
+        <f t="shared" si="17"/>
         <v>241500000</v>
       </c>
       <c r="L191" s="23">
         <v>0</v>
       </c>
       <c r="M191" s="25" t="str">
-        <f t="shared" si="33"/>
+        <f t="shared" si="31"/>
         <v>NÃO ASSISTIDO</v>
       </c>
       <c r="N191" s="6">
@@ -13211,14 +13091,14 @@
         <v>386000000</v>
       </c>
       <c r="K192" s="44">
-        <f t="shared" si="32"/>
+        <f t="shared" si="17"/>
         <v>251000000</v>
       </c>
       <c r="L192" s="23">
         <v>0</v>
       </c>
       <c r="M192" s="25" t="str">
-        <f t="shared" si="33"/>
+        <f t="shared" si="31"/>
         <v>NÃO ASSISTIDO</v>
       </c>
       <c r="N192" s="6">
@@ -13254,14 +13134,14 @@
         <v>347182886</v>
       </c>
       <c r="K193" s="44">
-        <f t="shared" si="32"/>
+        <f t="shared" si="17"/>
         <v>222182886</v>
       </c>
       <c r="L193" s="23">
         <v>0</v>
       </c>
       <c r="M193" s="25" t="str">
-        <f t="shared" si="33"/>
+        <f t="shared" si="31"/>
         <v>NÃO ASSISTIDO</v>
       </c>
       <c r="N193" s="6">
@@ -13297,14 +13177,14 @@
         <v>528000000</v>
       </c>
       <c r="K194" s="44">
-        <f t="shared" si="32"/>
+        <f t="shared" si="17"/>
         <v>418000000</v>
       </c>
       <c r="L194" s="23">
         <v>0</v>
       </c>
       <c r="M194" s="25" t="str">
-        <f t="shared" si="33"/>
+        <f t="shared" si="31"/>
         <v>NÃO ASSISTIDO</v>
       </c>
       <c r="N194" s="6">
@@ -13340,14 +13220,14 @@
         <v>125400000</v>
       </c>
       <c r="K195" s="44">
-        <f t="shared" si="32"/>
+        <f t="shared" ref="K195:K205" si="32">IF(OR(ISBLANK(J195),ISBLANK(I195)),"DESCONHECIDO",J195-I195)</f>
         <v>87400000</v>
       </c>
       <c r="L195" s="23">
         <v>0</v>
       </c>
       <c r="M195" s="25" t="str">
-        <f t="shared" si="33"/>
+        <f t="shared" si="31"/>
         <v>NÃO ASSISTIDO</v>
       </c>
       <c r="N195" s="6">
@@ -13390,7 +13270,7 @@
         <v>0</v>
       </c>
       <c r="M196" s="25" t="str">
-        <f t="shared" si="33"/>
+        <f t="shared" si="31"/>
         <v>NÃO ASSISTIDO</v>
       </c>
       <c r="N196" s="6">
@@ -13433,7 +13313,7 @@
         <v>0</v>
       </c>
       <c r="M197" s="25" t="str">
-        <f t="shared" si="33"/>
+        <f t="shared" si="31"/>
         <v>NÃO ASSISTIDO</v>
       </c>
       <c r="N197" s="6">
@@ -13476,7 +13356,7 @@
         <v>0</v>
       </c>
       <c r="M198" s="25" t="str">
-        <f t="shared" si="33"/>
+        <f t="shared" si="31"/>
         <v>NÃO ASSISTIDO</v>
       </c>
       <c r="N198" s="6">
@@ -13512,7 +13392,7 @@
         <v>216000000</v>
       </c>
       <c r="K199" s="44">
-        <f>J199-I199</f>
+        <f t="shared" si="32"/>
         <v>151000000</v>
       </c>
       <c r="L199" s="23">
@@ -13555,7 +13435,7 @@
         <v>42000000</v>
       </c>
       <c r="K200" s="44">
-        <f>J200-I200</f>
+        <f t="shared" si="32"/>
         <v>12000000</v>
       </c>
       <c r="L200" s="23">
@@ -13572,7 +13452,7 @@
     </row>
     <row r="201" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A201" s="6">
-        <f t="shared" si="20"/>
+        <f t="shared" ref="A201:A218" si="33">ROW()-1</f>
         <v>200</v>
       </c>
       <c r="B201" s="4" t="s">
@@ -13598,7 +13478,7 @@
         <v>146800000</v>
       </c>
       <c r="K201" s="44">
-        <f>J201-I201</f>
+        <f t="shared" si="32"/>
         <v>64800000</v>
       </c>
       <c r="L201" s="23">
@@ -13611,6 +13491,405 @@
       <c r="N201" s="6">
         <f t="shared" si="23"/>
         <v>200</v>
+      </c>
+    </row>
+    <row r="202" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A202" s="6">
+        <f t="shared" si="33"/>
+        <v>201</v>
+      </c>
+      <c r="B202" s="4" t="s">
+        <v>256</v>
+      </c>
+      <c r="C202" s="5">
+        <v>2018</v>
+      </c>
+      <c r="D202" s="6" t="s">
+        <v>257</v>
+      </c>
+      <c r="E202" s="7">
+        <v>45381</v>
+      </c>
+      <c r="F202" s="9">
+        <v>8</v>
+      </c>
+      <c r="G202" s="65">
+        <v>8.0555555555555561E-2</v>
+      </c>
+      <c r="H202" s="6" t="s">
+        <v>84</v>
+      </c>
+      <c r="I202" s="48">
+        <v>90000000</v>
+      </c>
+      <c r="J202" s="46">
+        <v>375500000</v>
+      </c>
+      <c r="K202" s="44">
+        <f t="shared" si="32"/>
+        <v>285500000</v>
+      </c>
+      <c r="L202" s="23">
+        <v>1</v>
+      </c>
+      <c r="M202" s="25" t="str">
+        <f>IF(ISBLANK(F202),"NÃO ASSISTIDO","ASSISTIDO")</f>
+        <v>ASSISTIDO</v>
+      </c>
+      <c r="N202" s="6">
+        <f t="shared" si="23"/>
+        <v>201</v>
+      </c>
+    </row>
+    <row r="203" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A203" s="6">
+        <f t="shared" si="33"/>
+        <v>202</v>
+      </c>
+      <c r="B203" s="4" t="s">
+        <v>258</v>
+      </c>
+      <c r="C203" s="5">
+        <v>2023</v>
+      </c>
+      <c r="D203" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="E203" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="F203" s="9">
+        <v>6</v>
+      </c>
+      <c r="G203" s="65">
+        <v>7.013888888888889E-2</v>
+      </c>
+      <c r="H203" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="I203" s="48">
+        <v>45000000</v>
+      </c>
+      <c r="J203" s="46">
+        <v>220000000</v>
+      </c>
+      <c r="K203" s="44">
+        <f t="shared" si="32"/>
+        <v>175000000</v>
+      </c>
+      <c r="L203" s="23">
+        <v>1</v>
+      </c>
+      <c r="M203" s="26" t="s">
+        <v>259</v>
+      </c>
+      <c r="N203" s="6">
+        <f t="shared" si="23"/>
+        <v>202</v>
+      </c>
+    </row>
+    <row r="204" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A204" s="6">
+        <f t="shared" si="33"/>
+        <v>203</v>
+      </c>
+      <c r="B204" s="4" t="s">
+        <v>260</v>
+      </c>
+      <c r="C204" s="5">
+        <v>2023</v>
+      </c>
+      <c r="D204" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="E204" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="F204" s="9">
+        <v>10</v>
+      </c>
+      <c r="G204" s="65">
+        <v>7.013888888888889E-2</v>
+      </c>
+      <c r="H204" s="6" t="s">
+        <v>261</v>
+      </c>
+      <c r="K204" s="44" t="str">
+        <f t="shared" si="32"/>
+        <v>DESCONHECIDO</v>
+      </c>
+      <c r="L204" s="23">
+        <v>1</v>
+      </c>
+      <c r="M204" s="26" t="s">
+        <v>259</v>
+      </c>
+      <c r="N204" s="6">
+        <f t="shared" si="23"/>
+        <v>203</v>
+      </c>
+    </row>
+    <row r="205" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A205" s="6">
+        <f t="shared" si="33"/>
+        <v>204</v>
+      </c>
+      <c r="B205" s="4" t="s">
+        <v>262</v>
+      </c>
+      <c r="C205" s="5">
+        <v>2024</v>
+      </c>
+      <c r="D205" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="E205" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="F205" s="9">
+        <v>7</v>
+      </c>
+      <c r="G205" s="65">
+        <v>6.458333333333334E-2</v>
+      </c>
+      <c r="H205" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="K205" s="44" t="str">
+        <f t="shared" si="32"/>
+        <v>DESCONHECIDO</v>
+      </c>
+      <c r="L205" s="23">
+        <v>1</v>
+      </c>
+      <c r="M205" s="26" t="s">
+        <v>259</v>
+      </c>
+      <c r="N205" s="6">
+        <f t="shared" si="23"/>
+        <v>204</v>
+      </c>
+    </row>
+    <row r="206" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A206" s="6">
+        <f t="shared" si="33"/>
+        <v>205</v>
+      </c>
+      <c r="B206" s="79"/>
+      <c r="K206" s="44">
+        <f t="shared" ref="K206:K218" si="34">J206-I206</f>
+        <v>0</v>
+      </c>
+      <c r="M206" s="26" t="s">
+        <v>259</v>
+      </c>
+      <c r="N206" s="6">
+        <f t="shared" si="23"/>
+        <v>205</v>
+      </c>
+    </row>
+    <row r="207" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A207" s="6">
+        <f t="shared" si="33"/>
+        <v>206</v>
+      </c>
+      <c r="K207" s="44">
+        <f t="shared" si="34"/>
+        <v>0</v>
+      </c>
+      <c r="M207" s="26" t="s">
+        <v>259</v>
+      </c>
+      <c r="N207" s="6">
+        <f t="shared" si="23"/>
+        <v>206</v>
+      </c>
+    </row>
+    <row r="208" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A208" s="6">
+        <f t="shared" si="33"/>
+        <v>207</v>
+      </c>
+      <c r="K208" s="44">
+        <f t="shared" si="34"/>
+        <v>0</v>
+      </c>
+      <c r="M208" s="26" t="s">
+        <v>259</v>
+      </c>
+      <c r="N208" s="6">
+        <f t="shared" si="23"/>
+        <v>207</v>
+      </c>
+    </row>
+    <row r="209" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A209" s="6">
+        <f t="shared" si="33"/>
+        <v>208</v>
+      </c>
+      <c r="K209" s="44">
+        <f t="shared" si="34"/>
+        <v>0</v>
+      </c>
+      <c r="M209" s="26" t="s">
+        <v>259</v>
+      </c>
+      <c r="N209" s="6">
+        <f t="shared" si="23"/>
+        <v>208</v>
+      </c>
+    </row>
+    <row r="210" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A210" s="6">
+        <f t="shared" si="33"/>
+        <v>209</v>
+      </c>
+      <c r="K210" s="44">
+        <f t="shared" si="34"/>
+        <v>0</v>
+      </c>
+      <c r="M210" s="26" t="s">
+        <v>259</v>
+      </c>
+      <c r="N210" s="6">
+        <f t="shared" si="23"/>
+        <v>209</v>
+      </c>
+    </row>
+    <row r="211" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A211" s="6">
+        <f t="shared" si="33"/>
+        <v>210</v>
+      </c>
+      <c r="K211" s="44">
+        <f t="shared" si="34"/>
+        <v>0</v>
+      </c>
+      <c r="M211" s="26" t="s">
+        <v>259</v>
+      </c>
+      <c r="N211" s="6">
+        <f t="shared" si="23"/>
+        <v>210</v>
+      </c>
+    </row>
+    <row r="212" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A212" s="6">
+        <f t="shared" si="33"/>
+        <v>211</v>
+      </c>
+      <c r="K212" s="44">
+        <f t="shared" si="34"/>
+        <v>0</v>
+      </c>
+      <c r="M212" s="26" t="s">
+        <v>259</v>
+      </c>
+      <c r="N212" s="6">
+        <f t="shared" si="23"/>
+        <v>211</v>
+      </c>
+    </row>
+    <row r="213" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A213" s="6">
+        <f t="shared" si="33"/>
+        <v>212</v>
+      </c>
+      <c r="K213" s="44">
+        <f t="shared" si="34"/>
+        <v>0</v>
+      </c>
+      <c r="M213" s="26" t="s">
+        <v>259</v>
+      </c>
+      <c r="N213" s="6">
+        <f t="shared" si="23"/>
+        <v>212</v>
+      </c>
+    </row>
+    <row r="214" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A214" s="6">
+        <f t="shared" si="33"/>
+        <v>213</v>
+      </c>
+      <c r="K214" s="44">
+        <f t="shared" si="34"/>
+        <v>0</v>
+      </c>
+      <c r="M214" s="26" t="s">
+        <v>259</v>
+      </c>
+      <c r="N214" s="6">
+        <f t="shared" si="23"/>
+        <v>213</v>
+      </c>
+    </row>
+    <row r="215" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A215" s="6">
+        <f t="shared" si="33"/>
+        <v>214</v>
+      </c>
+      <c r="K215" s="44">
+        <f t="shared" si="34"/>
+        <v>0</v>
+      </c>
+      <c r="M215" s="26" t="s">
+        <v>259</v>
+      </c>
+      <c r="N215" s="6">
+        <f t="shared" si="23"/>
+        <v>214</v>
+      </c>
+    </row>
+    <row r="216" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A216" s="6">
+        <f t="shared" si="33"/>
+        <v>215</v>
+      </c>
+      <c r="K216" s="44">
+        <f t="shared" si="34"/>
+        <v>0</v>
+      </c>
+      <c r="M216" s="26" t="s">
+        <v>259</v>
+      </c>
+      <c r="N216" s="6">
+        <f t="shared" ref="N216:N218" si="35">ROW()-1</f>
+        <v>215</v>
+      </c>
+    </row>
+    <row r="217" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A217" s="6">
+        <f t="shared" si="33"/>
+        <v>216</v>
+      </c>
+      <c r="K217" s="44">
+        <f t="shared" si="34"/>
+        <v>0</v>
+      </c>
+      <c r="M217" s="26" t="s">
+        <v>259</v>
+      </c>
+      <c r="N217" s="6">
+        <f t="shared" si="35"/>
+        <v>216</v>
+      </c>
+    </row>
+    <row r="218" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A218" s="6">
+        <f t="shared" si="33"/>
+        <v>217</v>
+      </c>
+      <c r="K218" s="44">
+        <f t="shared" si="34"/>
+        <v>0</v>
+      </c>
+      <c r="M218" s="26" t="s">
+        <v>259</v>
+      </c>
+      <c r="N218" s="6">
+        <f t="shared" si="35"/>
+        <v>217</v>
       </c>
     </row>
   </sheetData>
@@ -13621,72 +13900,77 @@
     <mergeCell ref="AC47:AE47"/>
   </mergeCells>
   <conditionalFormatting sqref="F1:F1048576">
-    <cfRule type="cellIs" dxfId="16" priority="15" operator="greaterThanOrEqual">
+    <cfRule type="cellIs" dxfId="34" priority="16" operator="greaterThanOrEqual">
       <formula>8</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="15" priority="16" operator="greaterThanOrEqual">
+    <cfRule type="cellIs" dxfId="33" priority="17" operator="greaterThanOrEqual">
       <formula>5</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="14" priority="17" operator="greaterThanOrEqual">
+    <cfRule type="cellIs" dxfId="32" priority="18" operator="greaterThanOrEqual">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K1:K1048576">
-    <cfRule type="cellIs" dxfId="13" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="31" priority="7" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K2:K1048576">
-    <cfRule type="cellIs" dxfId="12" priority="7" operator="lessThan">
+    <cfRule type="cellIs" dxfId="30" priority="8" operator="lessThan">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="11" priority="8" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="29" priority="9" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L1:L1048576">
-    <cfRule type="cellIs" dxfId="10" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="28" priority="6" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="R1:R36 Q20:Q21 M1:M1048576 U32:U1048576 R60:R1048576 Z1:Z1048576 AE1:AE46 AE48:AE1048576">
-    <cfRule type="cellIs" dxfId="9" priority="21" operator="equal">
+  <conditionalFormatting sqref="R1:R36 Q20:Q21 U32:U1048576 R60:R1048576 Z1:Z1048576 AE1:AE46 AE48:AE1048576 M1:M1048576">
+    <cfRule type="cellIs" dxfId="27" priority="22" operator="equal">
       <formula>"NÃO ASSISTIDO"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="8" priority="22" operator="equal">
+    <cfRule type="cellIs" dxfId="26" priority="23" operator="equal">
       <formula>"ASSISTIDO"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="U1:U30 Q12">
-    <cfRule type="cellIs" dxfId="7" priority="19" operator="equal">
+    <cfRule type="cellIs" dxfId="25" priority="20" operator="equal">
       <formula>"NÃO ASSISTIDO"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="6" priority="20" operator="equal">
+    <cfRule type="cellIs" dxfId="24" priority="21" operator="equal">
       <formula>"ASSISTIDO"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="V5">
-    <cfRule type="cellIs" dxfId="5" priority="13" operator="equal">
+    <cfRule type="cellIs" dxfId="23" priority="14" operator="equal">
       <formula>"NÃO ASSISTIDO"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="4" priority="14" operator="equal">
+    <cfRule type="cellIs" dxfId="22" priority="15" operator="equal">
       <formula>"ASSISTIDO"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AA5">
-    <cfRule type="cellIs" dxfId="3" priority="9" operator="equal">
+    <cfRule type="cellIs" dxfId="21" priority="10" operator="equal">
       <formula>"NÃO ASSISTIDO"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="10" operator="equal">
+    <cfRule type="cellIs" dxfId="20" priority="11" operator="equal">
       <formula>"ASSISTIDO"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AF5">
-    <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="19" priority="2" operator="equal">
       <formula>"NÃO ASSISTIDO"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="0" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="18" priority="3" operator="equal">
       <formula>"ASSISTIDO"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K2:K205">
+    <cfRule type="cellIs" dxfId="17" priority="1" operator="equal">
+      <formula>"DESCONHECIDO"</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>

</xml_diff>